<commit_message>
Calculated r with average daily temperatures
</commit_message>
<xml_diff>
--- a/Model results Tave.xlsx
+++ b/Model results Tave.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316E91A7-A799-5040-B776-8787AE1F2C01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71AF131-C6B9-3542-90F7-AC906A8DB89D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="6060" yWindow="500" windowWidth="22560" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -346,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,6 +524,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -736,7 +742,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -755,6 +761,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1113,7 +1120,7 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+      <selection activeCell="O6" sqref="O6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2024,7 +2031,7 @@
       <c r="G15" s="1">
         <v>0.154</v>
       </c>
-      <c r="H15" s="1">
+      <c r="H15" s="18">
         <v>1.25</v>
       </c>
       <c r="I15">

</xml_diff>

<commit_message>
Ran DDE model without density-dependence for all species to quantify r directly from population dynamics
</commit_message>
<xml_diff>
--- a/Model results Tave.xlsx
+++ b/Model results Tave.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9212FDED-63C5-C34A-9C24-146067C3EAB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{943FFEEA-EAB1-284A-9C5C-832EF097EE65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2400" yWindow="500" windowWidth="22560" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6200" yWindow="500" windowWidth="22560" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -170,15 +170,6 @@
     <t>Rhopalosiphum rufiabdominalis US Weston</t>
   </si>
   <si>
-    <t>delta.prop.TPC</t>
-  </si>
-  <si>
-    <t>delta.prop.model</t>
-  </si>
-  <si>
-    <t>rMax</t>
-  </si>
-  <si>
     <t>TPC historical</t>
   </si>
   <si>
@@ -189,6 +180,15 @@
   </si>
   <si>
     <t>Model future</t>
+  </si>
+  <si>
+    <t>rMax.TPC</t>
+  </si>
+  <si>
+    <t>rMax.model.f</t>
+  </si>
+  <si>
+    <t>rMax.model.h</t>
   </si>
 </sst>
 </file>
@@ -742,7 +742,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -762,11 +762,8 @@
     <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="19" fillId="33" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1125,19 +1122,19 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="52.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="44.83203125" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="15.1640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="13.5" customWidth="1"/>
+    <col min="7" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
@@ -1154,43 +1151,43 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>52</v>
+      </c>
+      <c r="G1" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>46</v>
+      </c>
+      <c r="I1" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="K1" s="12" t="s">
         <v>49</v>
       </c>
-      <c r="G1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="H1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="J1" s="13" t="s">
+      <c r="L1" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="12" t="s">
+      <c r="M1" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="N1" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="15" t="s">
+      <c r="O1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="P1" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="O1" s="12" t="s">
+      <c r="Q1" s="12" t="s">
         <v>29</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>47</v>
       </c>
       <c r="R1" s="13" t="s">
         <v>8</v>
@@ -1212,49 +1209,47 @@
       <c r="E2">
         <v>0.13400000000000001</v>
       </c>
-      <c r="F2" s="8">
+      <c r="F2">
         <v>0.127</v>
       </c>
-      <c r="G2" s="6">
+      <c r="G2">
+        <v>0.108</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0.127</v>
+      </c>
+      <c r="I2" s="6">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="H2" s="6">
+      <c r="J2" s="6">
         <v>0.12</v>
       </c>
-      <c r="I2" s="5">
+      <c r="K2" s="5">
         <v>7.5999999999999998E-2</v>
       </c>
-      <c r="J2" s="9">
-        <f>F2/$E2</f>
+      <c r="L2" s="9">
+        <f>H2/$E2</f>
         <v>0.94776119402985071</v>
       </c>
-      <c r="K2" s="14">
-        <f>G2/$E2</f>
+      <c r="M2" s="14">
+        <f>I2/$E2</f>
         <v>0.61940298507462688</v>
       </c>
-      <c r="L2" s="14">
-        <f>H2/$E2</f>
-        <v>0.89552238805970141</v>
-      </c>
-      <c r="M2" s="16">
-        <f>I2/$E2</f>
-        <v>0.56716417910447758</v>
-      </c>
-      <c r="N2" s="1">
-        <f>K2-J2</f>
-        <v>-0.32835820895522383</v>
-      </c>
-      <c r="O2" s="1">
+      <c r="N2" s="14">
+        <f>J2/$F2</f>
+        <v>0.94488188976377951</v>
+      </c>
+      <c r="O2" s="16">
+        <f>K2/$F2</f>
+        <v>0.59842519685039364</v>
+      </c>
+      <c r="P2" s="1">
         <f>M2-L2</f>
         <v>-0.32835820895522383</v>
       </c>
-      <c r="P2" s="10">
-        <f>(K2-J2)/J2</f>
-        <v>-0.34645669291338577</v>
-      </c>
       <c r="Q2" s="1">
-        <f>(M2-L2)/L2</f>
-        <v>-0.36666666666666664</v>
+        <f>O2-N2</f>
+        <v>-0.34645669291338588</v>
       </c>
       <c r="R2" s="7"/>
     </row>
@@ -1274,49 +1269,47 @@
       <c r="E3">
         <v>0.154</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3">
+        <v>0.13200000000000001</v>
+      </c>
+      <c r="G3">
+        <v>0.157</v>
+      </c>
+      <c r="H3" s="9">
         <v>0.125</v>
       </c>
-      <c r="G3" s="5">
+      <c r="I3" s="5">
         <v>0.152</v>
       </c>
-      <c r="H3" s="5">
+      <c r="J3" s="5">
         <v>0.11600000000000001</v>
       </c>
-      <c r="I3" s="5">
+      <c r="K3" s="5">
         <v>0.14799999999999999</v>
       </c>
-      <c r="J3" s="9">
-        <f t="shared" ref="J3:J28" si="0">F3/$E3</f>
+      <c r="L3" s="9">
+        <f t="shared" ref="L3:L28" si="0">H3/$E3</f>
         <v>0.81168831168831168</v>
       </c>
-      <c r="K3" s="14">
-        <f t="shared" ref="K3:K28" si="1">G3/$E3</f>
+      <c r="M3" s="14">
+        <f t="shared" ref="M3:M28" si="1">I3/$E3</f>
         <v>0.98701298701298701</v>
       </c>
-      <c r="L3" s="14">
-        <f t="shared" ref="L3:L28" si="2">H3/$E3</f>
-        <v>0.75324675324675328</v>
-      </c>
-      <c r="M3" s="16">
-        <f t="shared" ref="M3:M28" si="3">I3/$E3</f>
-        <v>0.96103896103896103</v>
-      </c>
-      <c r="N3" s="1">
-        <f t="shared" ref="N3:N28" si="4">K3-J3</f>
+      <c r="N3" s="14">
+        <f t="shared" ref="N3:N28" si="2">J3/$F3</f>
+        <v>0.87878787878787878</v>
+      </c>
+      <c r="O3" s="16">
+        <f t="shared" ref="O3:O28" si="3">K3/$F3</f>
+        <v>1.1212121212121211</v>
+      </c>
+      <c r="P3" s="1">
+        <f t="shared" ref="P3:P28" si="4">M3-L3</f>
         <v>0.17532467532467533</v>
       </c>
-      <c r="O3" s="1">
-        <f t="shared" ref="O3:O28" si="5">M3-L3</f>
-        <v>0.20779220779220775</v>
-      </c>
-      <c r="P3" s="10">
-        <f t="shared" ref="P3:P28" si="6">(K3-J3)/J3</f>
-        <v>0.216</v>
-      </c>
       <c r="Q3" s="1">
-        <f t="shared" ref="Q3:Q28" si="7">(M3-L3)/L3</f>
-        <v>0.27586206896551718</v>
+        <f t="shared" ref="Q3:Q28" si="5">O3-N3</f>
+        <v>0.24242424242424232</v>
       </c>
       <c r="R3" s="7"/>
     </row>
@@ -1336,49 +1329,47 @@
       <c r="E4">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4">
+        <v>0.182</v>
+      </c>
+      <c r="G4">
+        <v>0.19800000000000001</v>
+      </c>
+      <c r="H4" s="9">
         <v>7.9000000000000001E-2</v>
       </c>
-      <c r="G4" s="6">
+      <c r="I4" s="6">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="H4" s="22">
+      <c r="J4" s="5">
         <v>0.159</v>
       </c>
-      <c r="I4" s="19">
+      <c r="K4" s="6">
         <v>0.19400000000000001</v>
       </c>
-      <c r="J4" s="9">
+      <c r="L4" s="9">
         <f t="shared" si="0"/>
         <v>0.89772727272727282</v>
       </c>
-      <c r="K4" s="14">
+      <c r="M4" s="14">
         <f t="shared" si="1"/>
         <v>0.98863636363636365</v>
       </c>
-      <c r="L4" s="20">
+      <c r="N4" s="14">
         <f t="shared" si="2"/>
-        <v>1.8068181818181819</v>
-      </c>
-      <c r="M4" s="21">
+        <v>0.87362637362637363</v>
+      </c>
+      <c r="O4" s="16">
         <f t="shared" si="3"/>
-        <v>2.2045454545454546</v>
-      </c>
-      <c r="N4" s="1">
+        <v>1.0659340659340659</v>
+      </c>
+      <c r="P4" s="1">
         <f t="shared" si="4"/>
         <v>9.0909090909090828E-2</v>
       </c>
-      <c r="O4" s="1">
+      <c r="Q4" s="1">
         <f t="shared" si="5"/>
-        <v>0.39772727272727271</v>
-      </c>
-      <c r="P4" s="10">
-        <f t="shared" si="6"/>
-        <v>0.10126582278481003</v>
-      </c>
-      <c r="Q4" s="1">
-        <f t="shared" si="7"/>
-        <v>0.22012578616352199</v>
+        <v>0.19230769230769229</v>
       </c>
       <c r="R4" s="7"/>
     </row>
@@ -1398,49 +1389,47 @@
       <c r="E5">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5">
+        <v>0.104</v>
+      </c>
+      <c r="G5">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="H5" s="8">
         <v>8.1000000000000003E-2</v>
       </c>
-      <c r="G5" s="6">
+      <c r="I5" s="6">
         <v>8.2000000000000003E-2</v>
       </c>
-      <c r="H5" s="6">
+      <c r="J5" s="6">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="I5" s="6">
+      <c r="K5" s="6">
         <v>4.9000000000000002E-2</v>
       </c>
-      <c r="J5" s="9">
+      <c r="L5" s="9">
         <f t="shared" si="0"/>
         <v>0.92045454545454553</v>
       </c>
-      <c r="K5" s="14">
+      <c r="M5" s="14">
         <f t="shared" si="1"/>
         <v>0.93181818181818188</v>
       </c>
-      <c r="L5" s="14">
+      <c r="N5" s="14">
         <f t="shared" si="2"/>
-        <v>1.0340909090909092</v>
-      </c>
-      <c r="M5" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="O5" s="16">
         <f t="shared" si="3"/>
-        <v>0.55681818181818188</v>
-      </c>
-      <c r="N5" s="1">
+        <v>0.4711538461538462</v>
+      </c>
+      <c r="P5" s="1">
         <f t="shared" si="4"/>
         <v>1.1363636363636354E-2</v>
       </c>
-      <c r="O5" s="1">
+      <c r="Q5" s="1">
         <f t="shared" si="5"/>
-        <v>-0.47727272727272729</v>
-      </c>
-      <c r="P5" s="10">
-        <f t="shared" si="6"/>
-        <v>1.2345679012345668E-2</v>
-      </c>
-      <c r="Q5" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.46153846153846151</v>
+        <v>-0.4038461538461538</v>
       </c>
       <c r="R5" s="7"/>
     </row>
@@ -1460,49 +1449,47 @@
       <c r="E6">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6">
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.106</v>
+      </c>
+      <c r="H6" s="9">
         <v>0.104</v>
       </c>
-      <c r="G6" s="6">
+      <c r="I6" s="6">
         <v>0.109</v>
       </c>
-      <c r="H6" s="5">
+      <c r="J6" s="5">
         <v>0.10199999999999999</v>
       </c>
-      <c r="I6" s="6">
+      <c r="K6" s="6">
         <v>0.10100000000000001</v>
       </c>
-      <c r="J6" s="9">
-        <f t="shared" si="0"/>
+      <c r="L6" s="9">
+        <f>H6/$E6</f>
         <v>0.63030303030303025</v>
       </c>
-      <c r="K6" s="14">
-        <f t="shared" si="1"/>
+      <c r="M6" s="14">
+        <f>I6/$E6</f>
         <v>0.66060606060606053</v>
       </c>
-      <c r="L6" s="14">
-        <f t="shared" si="2"/>
-        <v>0.61818181818181817</v>
-      </c>
-      <c r="M6" s="16">
-        <f t="shared" si="3"/>
-        <v>0.61212121212121218</v>
-      </c>
-      <c r="N6" s="1">
+      <c r="N6" s="14">
+        <f>J6/$F6</f>
+        <v>0.73913043478260854</v>
+      </c>
+      <c r="O6" s="16">
+        <f>K6/$F6</f>
+        <v>0.73188405797101452</v>
+      </c>
+      <c r="P6" s="1">
         <f t="shared" si="4"/>
         <v>3.0303030303030276E-2</v>
       </c>
-      <c r="O6" s="1">
+      <c r="Q6" s="1">
         <f t="shared" si="5"/>
-        <v>-6.0606060606059886E-3</v>
-      </c>
-      <c r="P6" s="10">
-        <f t="shared" si="6"/>
-        <v>4.8076923076923038E-2</v>
-      </c>
-      <c r="Q6" s="1">
-        <f t="shared" si="7"/>
-        <v>-9.8039215686273346E-3</v>
+        <v>-7.246376811594013E-3</v>
       </c>
       <c r="R6" s="7" t="s">
         <v>27</v>
@@ -1524,49 +1511,47 @@
       <c r="E7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7">
+        <v>0.155</v>
+      </c>
+      <c r="G7">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="H7" s="9">
         <v>5.1999999999999998E-2</v>
       </c>
-      <c r="G7" s="6">
+      <c r="I7" s="6">
         <v>6.3E-2</v>
       </c>
-      <c r="H7" s="5">
+      <c r="J7" s="5">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="I7" s="6">
+      <c r="K7" s="6">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="J7" s="9">
+      <c r="L7" s="9">
         <f t="shared" si="0"/>
         <v>0.62650602409638545</v>
       </c>
-      <c r="K7" s="14">
+      <c r="M7" s="14">
         <f t="shared" si="1"/>
         <v>0.75903614457831325</v>
       </c>
-      <c r="L7" s="14">
+      <c r="N7" s="14">
         <f t="shared" si="2"/>
-        <v>1.0963855421686746</v>
-      </c>
-      <c r="M7" s="16">
+        <v>0.58709677419354833</v>
+      </c>
+      <c r="O7" s="16">
         <f t="shared" si="3"/>
-        <v>1.0240963855421688</v>
-      </c>
-      <c r="N7" s="1">
+        <v>0.54838709677419362</v>
+      </c>
+      <c r="P7" s="1">
         <f t="shared" si="4"/>
         <v>0.1325301204819278</v>
       </c>
-      <c r="O7" s="1">
+      <c r="Q7" s="1">
         <f t="shared" si="5"/>
-        <v>-7.2289156626505813E-2</v>
-      </c>
-      <c r="P7" s="10">
-        <f t="shared" si="6"/>
-        <v>0.21153846153846173</v>
-      </c>
-      <c r="Q7" s="1">
-        <f t="shared" si="7"/>
-        <v>-6.5934065934065755E-2</v>
+        <v>-3.8709677419354716E-2</v>
       </c>
       <c r="R7" s="7" t="s">
         <v>27</v>
@@ -1588,49 +1573,47 @@
       <c r="E8">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8">
+        <v>0.219</v>
+      </c>
+      <c r="G8">
+        <v>0.29599999999999999</v>
+      </c>
+      <c r="H8" s="8">
         <v>0.105</v>
       </c>
-      <c r="G8" s="6">
+      <c r="I8" s="6">
         <v>0.11600000000000001</v>
       </c>
-      <c r="H8" s="5">
+      <c r="J8" s="5">
         <v>0.16500000000000001</v>
       </c>
-      <c r="I8" s="5">
+      <c r="K8" s="5">
         <v>0.22700000000000001</v>
       </c>
-      <c r="J8" s="9">
+      <c r="L8" s="9">
         <f t="shared" si="0"/>
         <v>0.63636363636363635</v>
       </c>
-      <c r="K8" s="14">
+      <c r="M8" s="14">
         <f t="shared" si="1"/>
         <v>0.70303030303030301</v>
       </c>
-      <c r="L8" s="14">
+      <c r="N8" s="14">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="M8" s="16">
+        <v>0.75342465753424659</v>
+      </c>
+      <c r="O8" s="16">
         <f t="shared" si="3"/>
-        <v>1.3757575757575757</v>
-      </c>
-      <c r="N8" s="1">
+        <v>1.0365296803652968</v>
+      </c>
+      <c r="P8" s="1">
         <f t="shared" si="4"/>
         <v>6.6666666666666652E-2</v>
       </c>
-      <c r="O8" s="1">
+      <c r="Q8" s="1">
         <f t="shared" si="5"/>
-        <v>0.37575757575757573</v>
-      </c>
-      <c r="P8" s="10">
-        <f t="shared" si="6"/>
-        <v>0.10476190476190474</v>
-      </c>
-      <c r="Q8" s="1">
-        <f t="shared" si="7"/>
-        <v>0.37575757575757573</v>
+        <v>0.28310502283105021</v>
       </c>
       <c r="R8" s="7" t="s">
         <v>27</v>
@@ -1652,49 +1635,47 @@
       <c r="E9">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9">
+        <v>0.17799999999999999</v>
+      </c>
+      <c r="G9" s="1">
+        <v>0.16</v>
+      </c>
+      <c r="H9" s="9">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="G9" s="6">
+      <c r="I9" s="6">
         <v>5.3999999999999999E-2</v>
       </c>
-      <c r="H9" s="5">
+      <c r="J9" s="5">
         <v>0.107</v>
       </c>
-      <c r="I9" s="5">
+      <c r="K9" s="5">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="J9" s="9">
+      <c r="L9" s="9">
         <f t="shared" si="0"/>
         <v>0.6506024096385542</v>
       </c>
-      <c r="K9" s="14">
+      <c r="M9" s="14">
         <f t="shared" si="1"/>
         <v>0.6506024096385542</v>
       </c>
-      <c r="L9" s="14">
+      <c r="N9" s="14">
         <f t="shared" si="2"/>
-        <v>1.2891566265060239</v>
-      </c>
-      <c r="M9" s="16">
+        <v>0.601123595505618</v>
+      </c>
+      <c r="O9" s="16">
         <f t="shared" si="3"/>
-        <v>1.1204819277108433</v>
-      </c>
-      <c r="N9" s="1">
+        <v>0.52247191011235961</v>
+      </c>
+      <c r="P9" s="1">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="O9" s="1">
+      <c r="Q9" s="1">
         <f t="shared" si="5"/>
-        <v>-0.1686746987951806</v>
-      </c>
-      <c r="P9" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="Q9" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.13084112149532703</v>
+        <v>-7.8651685393258397E-2</v>
       </c>
       <c r="R9" s="7" t="s">
         <v>27</v>
@@ -1716,49 +1697,47 @@
       <c r="E10">
         <v>0.246</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="1">
+        <v>0.69</v>
+      </c>
+      <c r="G10">
+        <v>0.67600000000000005</v>
+      </c>
+      <c r="H10" s="9">
         <v>0.23400000000000001</v>
       </c>
-      <c r="G10" s="6">
+      <c r="I10" s="6">
         <v>0.215</v>
       </c>
-      <c r="H10" s="19">
+      <c r="J10" s="6">
         <v>0.66</v>
       </c>
-      <c r="I10" s="22">
+      <c r="K10" s="5">
         <v>0.46400000000000002</v>
       </c>
-      <c r="J10" s="9">
+      <c r="L10" s="9">
         <f t="shared" si="0"/>
         <v>0.95121951219512202</v>
       </c>
-      <c r="K10" s="14">
+      <c r="M10" s="14">
         <f t="shared" si="1"/>
         <v>0.87398373983739841</v>
       </c>
-      <c r="L10" s="20">
+      <c r="N10" s="14">
         <f t="shared" si="2"/>
-        <v>2.6829268292682928</v>
-      </c>
-      <c r="M10" s="21">
+        <v>0.95652173913043492</v>
+      </c>
+      <c r="O10" s="16">
         <f t="shared" si="3"/>
-        <v>1.8861788617886179</v>
-      </c>
-      <c r="N10" s="1">
+        <v>0.67246376811594211</v>
+      </c>
+      <c r="P10" s="1">
         <f t="shared" si="4"/>
         <v>-7.7235772357723609E-2</v>
       </c>
-      <c r="O10" s="1">
+      <c r="Q10" s="1">
         <f t="shared" si="5"/>
-        <v>-0.79674796747967491</v>
-      </c>
-      <c r="P10" s="10">
-        <f t="shared" si="6"/>
-        <v>-8.1196581196581227E-2</v>
-      </c>
-      <c r="Q10" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.29696969696969699</v>
+        <v>-0.28405797101449282</v>
       </c>
       <c r="R10" s="7"/>
     </row>
@@ -1778,49 +1757,47 @@
       <c r="E11">
         <v>0.25700000000000001</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="G11">
+        <v>0.69499999999999995</v>
+      </c>
+      <c r="H11" s="9">
         <v>0.24099999999999999</v>
       </c>
-      <c r="G11" s="6">
+      <c r="I11" s="6">
         <v>0.19600000000000001</v>
       </c>
-      <c r="H11" s="19">
+      <c r="J11" s="6">
         <v>0.68400000000000005</v>
       </c>
-      <c r="I11" s="19">
+      <c r="K11" s="6">
         <v>0.379</v>
       </c>
-      <c r="J11" s="9">
+      <c r="L11" s="9">
         <f t="shared" si="0"/>
         <v>0.9377431906614786</v>
       </c>
-      <c r="K11" s="14">
+      <c r="M11" s="14">
         <f t="shared" si="1"/>
         <v>0.76264591439688723</v>
       </c>
-      <c r="L11" s="20">
+      <c r="N11" s="14">
         <f t="shared" si="2"/>
-        <v>2.6614785992217902</v>
-      </c>
-      <c r="M11" s="21">
+        <v>0.94736842105263164</v>
+      </c>
+      <c r="O11" s="16">
         <f t="shared" si="3"/>
-        <v>1.4747081712062255</v>
-      </c>
-      <c r="N11" s="1">
+        <v>0.52493074792243766</v>
+      </c>
+      <c r="P11" s="1">
         <f t="shared" si="4"/>
         <v>-0.17509727626459137</v>
       </c>
-      <c r="O11" s="1">
+      <c r="Q11" s="1">
         <f t="shared" si="5"/>
-        <v>-1.1867704280155646</v>
-      </c>
-      <c r="P11" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.18672199170124473</v>
-      </c>
-      <c r="Q11" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.44590643274853814</v>
+        <v>-0.42243767313019398</v>
       </c>
       <c r="R11" s="7"/>
     </row>
@@ -1840,49 +1817,47 @@
       <c r="E12">
         <v>0.249</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F12">
+        <v>0.78100000000000003</v>
+      </c>
+      <c r="G12">
+        <v>0.77400000000000002</v>
+      </c>
+      <c r="H12" s="8">
         <v>0.23100000000000001</v>
       </c>
-      <c r="G12" s="6">
+      <c r="I12" s="6">
         <v>0.19700000000000001</v>
       </c>
-      <c r="H12" s="19">
+      <c r="J12" s="6">
         <v>0.73599999999999999</v>
       </c>
-      <c r="I12" s="22">
+      <c r="K12" s="5">
         <v>0.54700000000000004</v>
       </c>
-      <c r="J12" s="9">
+      <c r="L12" s="9">
         <f t="shared" si="0"/>
         <v>0.92771084337349408</v>
       </c>
-      <c r="K12" s="14">
+      <c r="M12" s="14">
         <f t="shared" si="1"/>
         <v>0.79116465863453822</v>
       </c>
-      <c r="L12" s="20">
+      <c r="N12" s="14">
         <f t="shared" si="2"/>
-        <v>2.9558232931726907</v>
-      </c>
-      <c r="M12" s="21">
+        <v>0.94238156209987189</v>
+      </c>
+      <c r="O12" s="16">
         <f t="shared" si="3"/>
-        <v>2.1967871485943777</v>
-      </c>
-      <c r="N12" s="1">
+        <v>0.70038412291933416</v>
+      </c>
+      <c r="P12" s="1">
         <f t="shared" si="4"/>
         <v>-0.13654618473895586</v>
       </c>
-      <c r="O12" s="1">
+      <c r="Q12" s="1">
         <f t="shared" si="5"/>
-        <v>-0.75903614457831292</v>
-      </c>
-      <c r="P12" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.1471861471861472</v>
-      </c>
-      <c r="Q12" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.25679347826086946</v>
+        <v>-0.24199743918053773</v>
       </c>
       <c r="R12" s="7"/>
     </row>
@@ -1902,49 +1877,47 @@
       <c r="E13" s="1">
         <v>0.1</v>
       </c>
-      <c r="F13" s="10">
+      <c r="F13" s="1">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G13" s="1">
+        <v>0.192</v>
+      </c>
+      <c r="H13" s="10">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="G13" s="1">
+      <c r="I13" s="1">
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="H13" s="1">
+      <c r="J13" s="3">
         <v>8.4000000000000005E-2</v>
       </c>
-      <c r="I13" s="4">
+      <c r="K13" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="J13" s="9">
+      <c r="L13" s="9">
         <f t="shared" si="0"/>
         <v>0.59</v>
       </c>
-      <c r="K13" s="14">
+      <c r="M13" s="14">
         <f t="shared" si="1"/>
         <v>0.34</v>
       </c>
-      <c r="L13" s="14">
+      <c r="N13" s="14">
         <f t="shared" si="2"/>
-        <v>0.84</v>
-      </c>
-      <c r="M13" s="16">
+        <v>0.6</v>
+      </c>
+      <c r="O13" s="16">
         <f t="shared" si="3"/>
-        <v>0.74999999999999989</v>
-      </c>
-      <c r="N13" s="1">
+        <v>0.5357142857142857</v>
+      </c>
+      <c r="P13" s="1">
         <f t="shared" si="4"/>
         <v>-0.24999999999999994</v>
       </c>
-      <c r="O13" s="1">
+      <c r="Q13" s="1">
         <f t="shared" si="5"/>
-        <v>-9.000000000000008E-2</v>
-      </c>
-      <c r="P13" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.42372881355932196</v>
-      </c>
-      <c r="Q13" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.10714285714285725</v>
+        <v>-6.4285714285714279E-2</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>27</v>
@@ -1966,49 +1939,47 @@
       <c r="E14">
         <v>0.104</v>
       </c>
-      <c r="F14" s="10">
+      <c r="F14">
+        <v>0.14799999999999999</v>
+      </c>
+      <c r="G14">
+        <v>0.19900000000000001</v>
+      </c>
+      <c r="H14" s="10">
         <v>5.8999999999999997E-2</v>
       </c>
-      <c r="G14" s="1">
+      <c r="I14" s="1">
         <v>0</v>
       </c>
-      <c r="H14" s="1">
+      <c r="J14" s="3">
         <v>8.6999999999999994E-2</v>
       </c>
-      <c r="I14" s="4">
+      <c r="K14" s="4">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="J14" s="9">
+      <c r="L14" s="9">
         <f t="shared" si="0"/>
         <v>0.56730769230769229</v>
       </c>
-      <c r="K14" s="14">
+      <c r="M14" s="14">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L14" s="14">
+      <c r="N14" s="14">
         <f t="shared" si="2"/>
-        <v>0.83653846153846156</v>
-      </c>
-      <c r="M14" s="16">
+        <v>0.58783783783783783</v>
+      </c>
+      <c r="O14" s="16">
         <f t="shared" si="3"/>
-        <v>0.72115384615384615</v>
-      </c>
-      <c r="N14" s="1">
+        <v>0.5067567567567568</v>
+      </c>
+      <c r="P14" s="1">
         <f t="shared" si="4"/>
         <v>-0.56730769230769229</v>
       </c>
-      <c r="O14" s="1">
+      <c r="Q14" s="1">
         <f t="shared" si="5"/>
-        <v>-0.11538461538461542</v>
-      </c>
-      <c r="P14" s="10">
-        <f t="shared" si="6"/>
-        <v>-1</v>
-      </c>
-      <c r="Q14" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.13793103448275865</v>
+        <v>-8.108108108108103E-2</v>
       </c>
       <c r="R14" s="7" t="s">
         <v>27</v>
@@ -2030,49 +2001,47 @@
       <c r="E15">
         <v>0.28599999999999998</v>
       </c>
-      <c r="F15" s="10">
+      <c r="F15">
+        <v>0.44900000000000001</v>
+      </c>
+      <c r="G15">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="H15" s="10">
         <v>0.124</v>
       </c>
-      <c r="G15" s="1">
+      <c r="I15" s="1">
         <v>0.154</v>
       </c>
-      <c r="H15" s="3">
+      <c r="J15" s="3">
         <v>0.25700000000000001</v>
       </c>
-      <c r="I15">
+      <c r="K15" s="4">
         <v>0.16200000000000001</v>
       </c>
-      <c r="J15" s="9">
+      <c r="L15" s="9">
         <f t="shared" si="0"/>
         <v>0.4335664335664336</v>
       </c>
-      <c r="K15" s="14">
+      <c r="M15" s="14">
         <f t="shared" si="1"/>
         <v>0.53846153846153855</v>
       </c>
-      <c r="L15" s="14">
+      <c r="N15" s="14">
         <f t="shared" si="2"/>
-        <v>0.89860139860139865</v>
-      </c>
-      <c r="M15" s="16">
+        <v>0.57238307349665929</v>
+      </c>
+      <c r="O15" s="16">
         <f t="shared" si="3"/>
-        <v>0.56643356643356646</v>
-      </c>
-      <c r="N15" s="1">
+        <v>0.36080178173719379</v>
+      </c>
+      <c r="P15" s="1">
         <f t="shared" si="4"/>
         <v>0.10489510489510495</v>
       </c>
-      <c r="O15" s="3">
+      <c r="Q15" s="3">
         <f t="shared" si="5"/>
-        <v>-0.33216783216783219</v>
-      </c>
-      <c r="P15" s="10">
-        <f t="shared" si="6"/>
-        <v>0.24193548387096786</v>
-      </c>
-      <c r="Q15" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.36964980544747084</v>
+        <v>-0.2115812917594655</v>
       </c>
       <c r="R15" s="7" t="s">
         <v>27</v>
@@ -2094,49 +2063,47 @@
       <c r="E16">
         <v>0.19400000000000001</v>
       </c>
-      <c r="F16" s="10">
+      <c r="F16">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G16">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="H16" s="10">
         <v>0.161</v>
       </c>
-      <c r="G16" s="1">
+      <c r="I16" s="1">
         <v>0.17499999999999999</v>
       </c>
-      <c r="H16" s="1">
+      <c r="J16" s="3">
         <v>0.109</v>
       </c>
-      <c r="I16">
+      <c r="K16" s="4">
         <v>0.10199999999999999</v>
       </c>
-      <c r="J16" s="9">
+      <c r="L16" s="9">
         <f t="shared" si="0"/>
         <v>0.82989690721649489</v>
       </c>
-      <c r="K16" s="14">
+      <c r="M16" s="14">
         <f t="shared" si="1"/>
         <v>0.902061855670103</v>
       </c>
-      <c r="L16" s="14">
+      <c r="N16" s="14">
         <f t="shared" si="2"/>
-        <v>0.56185567010309279</v>
-      </c>
-      <c r="M16" s="16">
+        <v>0.80147058823529405</v>
+      </c>
+      <c r="O16" s="16">
         <f t="shared" si="3"/>
-        <v>0.52577319587628857</v>
-      </c>
-      <c r="N16" s="1">
+        <v>0.74999999999999989</v>
+      </c>
+      <c r="P16" s="1">
         <f t="shared" si="4"/>
         <v>7.2164948453608102E-2</v>
       </c>
-      <c r="O16" s="1">
+      <c r="Q16" s="1">
         <f t="shared" si="5"/>
-        <v>-3.6082474226804218E-2</v>
-      </c>
-      <c r="P16" s="10">
-        <f t="shared" si="6"/>
-        <v>8.6956521739130252E-2</v>
-      </c>
-      <c r="Q16" s="1">
-        <f t="shared" si="7"/>
-        <v>-6.4220183486238702E-2</v>
+        <v>-5.1470588235294157E-2</v>
       </c>
       <c r="R16" s="7" t="s">
         <v>27</v>
@@ -2158,49 +2125,47 @@
       <c r="E17">
         <v>0.443</v>
       </c>
-      <c r="F17" s="10">
+      <c r="F17">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="G17">
+        <v>0.249</v>
+      </c>
+      <c r="H17" s="10">
         <v>0.40699999999999997</v>
       </c>
-      <c r="G17" s="1">
+      <c r="I17" s="1">
         <v>0.378</v>
       </c>
-      <c r="H17" s="1">
+      <c r="J17" s="3">
         <v>0.26400000000000001</v>
       </c>
-      <c r="I17" s="4">
+      <c r="K17" s="4">
         <v>0.124</v>
       </c>
-      <c r="J17" s="9">
+      <c r="L17" s="9">
         <f t="shared" si="0"/>
         <v>0.91873589164785541</v>
       </c>
-      <c r="K17" s="14">
+      <c r="M17" s="14">
         <f t="shared" si="1"/>
         <v>0.85327313769751689</v>
       </c>
-      <c r="L17" s="14">
+      <c r="N17" s="14">
         <f t="shared" si="2"/>
-        <v>0.59593679458239279</v>
-      </c>
-      <c r="M17" s="16">
+        <v>0.93286219081272093</v>
+      </c>
+      <c r="O17" s="16">
         <f t="shared" si="3"/>
-        <v>0.27990970654627539</v>
-      </c>
-      <c r="N17" s="1">
+        <v>0.43816254416961137</v>
+      </c>
+      <c r="P17" s="1">
         <f t="shared" si="4"/>
         <v>-6.5462753950338515E-2</v>
       </c>
-      <c r="O17" s="1">
+      <c r="Q17" s="1">
         <f t="shared" si="5"/>
-        <v>-0.3160270880361174</v>
-      </c>
-      <c r="P17" s="10">
-        <f t="shared" si="6"/>
-        <v>-7.1253071253071176E-2</v>
-      </c>
-      <c r="Q17" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.53030303030303028</v>
+        <v>-0.49469964664310956</v>
       </c>
       <c r="R17" s="7" t="s">
         <v>27</v>
@@ -2222,49 +2187,47 @@
       <c r="E18">
         <v>0.30599999999999999</v>
       </c>
-      <c r="F18" s="10">
+      <c r="F18">
+        <v>0.24099999999999999</v>
+      </c>
+      <c r="G18">
+        <v>0.217</v>
+      </c>
+      <c r="H18" s="10">
         <v>0.27</v>
       </c>
-      <c r="G18" s="1">
+      <c r="I18" s="1">
         <v>0.27200000000000002</v>
       </c>
-      <c r="H18" s="1">
+      <c r="J18" s="3">
         <v>0.215</v>
       </c>
-      <c r="I18" s="1">
+      <c r="K18" s="3">
         <v>0.19900000000000001</v>
       </c>
-      <c r="J18" s="9">
+      <c r="L18" s="9">
         <f t="shared" si="0"/>
         <v>0.88235294117647067</v>
       </c>
-      <c r="K18" s="14">
+      <c r="M18" s="14">
         <f t="shared" si="1"/>
         <v>0.88888888888888895</v>
       </c>
-      <c r="L18" s="14">
+      <c r="N18" s="14">
         <f t="shared" si="2"/>
-        <v>0.70261437908496738</v>
-      </c>
-      <c r="M18" s="16">
+        <v>0.89211618257261416</v>
+      </c>
+      <c r="O18" s="16">
         <f t="shared" si="3"/>
-        <v>0.65032679738562094</v>
-      </c>
-      <c r="N18" s="1">
+        <v>0.82572614107883824</v>
+      </c>
+      <c r="P18" s="1">
         <f t="shared" si="4"/>
         <v>6.5359477124182774E-3</v>
       </c>
-      <c r="O18" s="1">
+      <c r="Q18" s="1">
         <f t="shared" si="5"/>
-        <v>-5.2287581699346442E-2</v>
-      </c>
-      <c r="P18" s="10">
-        <f t="shared" si="6"/>
-        <v>7.4074074074073808E-3</v>
-      </c>
-      <c r="Q18" s="1">
-        <f t="shared" si="7"/>
-        <v>-7.4418604651162831E-2</v>
+        <v>-6.639004149377592E-2</v>
       </c>
       <c r="R18" s="7" t="s">
         <v>27</v>
@@ -2286,49 +2249,47 @@
       <c r="E19">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F19" s="10">
+      <c r="F19">
+        <v>0.188</v>
+      </c>
+      <c r="G19">
         <v>0.158</v>
       </c>
-      <c r="G19" s="1">
+      <c r="H19" s="10">
+        <v>0.158</v>
+      </c>
+      <c r="I19" s="1">
         <v>0.123</v>
       </c>
-      <c r="H19" s="1">
+      <c r="J19" s="3">
         <v>0.13600000000000001</v>
       </c>
-      <c r="I19">
+      <c r="K19" s="4">
         <v>0.104</v>
       </c>
-      <c r="J19" s="9">
+      <c r="L19" s="9">
         <f t="shared" si="0"/>
         <v>0.79396984924623115</v>
       </c>
-      <c r="K19" s="14">
+      <c r="M19" s="14">
         <f t="shared" si="1"/>
         <v>0.61809045226130654</v>
       </c>
-      <c r="L19" s="14">
+      <c r="N19" s="14">
         <f t="shared" si="2"/>
-        <v>0.68341708542713564</v>
-      </c>
-      <c r="M19" s="16">
+        <v>0.72340425531914898</v>
+      </c>
+      <c r="O19" s="16">
         <f t="shared" si="3"/>
-        <v>0.5226130653266331</v>
-      </c>
-      <c r="N19" s="1">
+        <v>0.55319148936170215</v>
+      </c>
+      <c r="P19" s="1">
         <f t="shared" si="4"/>
         <v>-0.17587939698492461</v>
       </c>
-      <c r="O19" s="1">
+      <c r="Q19" s="1">
         <f t="shared" si="5"/>
-        <v>-0.16080402010050254</v>
-      </c>
-      <c r="P19" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.22151898734177214</v>
-      </c>
-      <c r="Q19" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.23529411764705888</v>
+        <v>-0.17021276595744683</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>27</v>
@@ -2350,49 +2311,47 @@
       <c r="E20">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20">
+        <v>0.183</v>
+      </c>
+      <c r="G20">
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="H20" s="10">
         <v>0.14199999999999999</v>
       </c>
-      <c r="G20" s="1">
+      <c r="I20" s="1">
         <v>0.107</v>
       </c>
-      <c r="H20" s="1">
+      <c r="J20" s="3">
         <v>0.13700000000000001</v>
       </c>
-      <c r="I20">
+      <c r="K20" s="4">
         <v>9.1999999999999998E-2</v>
       </c>
-      <c r="J20" s="9">
+      <c r="L20" s="9">
         <f t="shared" si="0"/>
         <v>0.69607843137254899</v>
       </c>
-      <c r="K20" s="14">
+      <c r="M20" s="14">
         <f t="shared" si="1"/>
         <v>0.52450980392156865</v>
       </c>
-      <c r="L20" s="14">
+      <c r="N20" s="14">
         <f t="shared" si="2"/>
-        <v>0.67156862745098045</v>
-      </c>
-      <c r="M20" s="16">
+        <v>0.74863387978142082</v>
+      </c>
+      <c r="O20" s="16">
         <f t="shared" si="3"/>
-        <v>0.45098039215686275</v>
-      </c>
-      <c r="N20" s="1">
+        <v>0.50273224043715847</v>
+      </c>
+      <c r="P20" s="1">
         <f t="shared" si="4"/>
         <v>-0.17156862745098034</v>
       </c>
-      <c r="O20" s="1">
+      <c r="Q20" s="1">
         <f t="shared" si="5"/>
-        <v>-0.2205882352941177</v>
-      </c>
-      <c r="P20" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.24647887323943654</v>
-      </c>
-      <c r="Q20" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.32846715328467158</v>
+        <v>-0.24590163934426235</v>
       </c>
       <c r="R20" s="7" t="s">
         <v>27</v>
@@ -2414,49 +2373,47 @@
       <c r="E21">
         <v>1.49</v>
       </c>
-      <c r="F21" s="17">
+      <c r="F21">
+        <v>2.66</v>
+      </c>
+      <c r="G21">
+        <v>-2.1999999999999999E-2</v>
+      </c>
+      <c r="H21" s="17">
         <v>1.08</v>
       </c>
-      <c r="G21" s="3">
+      <c r="I21" s="3">
         <v>0.59199999999999997</v>
       </c>
-      <c r="H21" s="23">
+      <c r="J21" s="20">
         <v>1.69</v>
       </c>
-      <c r="I21" s="4">
+      <c r="K21" s="4">
         <v>-0.38400000000000001</v>
       </c>
-      <c r="J21" s="9">
+      <c r="L21" s="9">
         <f t="shared" si="0"/>
         <v>0.72483221476510074</v>
       </c>
-      <c r="K21" s="14">
+      <c r="M21" s="14">
         <f t="shared" si="1"/>
         <v>0.3973154362416107</v>
       </c>
-      <c r="L21" s="20">
+      <c r="N21" s="14">
         <f t="shared" si="2"/>
-        <v>1.1342281879194631</v>
-      </c>
-      <c r="M21" s="16">
+        <v>0.63533834586466165</v>
+      </c>
+      <c r="O21" s="16">
         <f t="shared" si="3"/>
-        <v>-0.25771812080536916</v>
-      </c>
-      <c r="N21" s="1">
-        <f>K21-J21</f>
+        <v>-0.14436090225563911</v>
+      </c>
+      <c r="P21" s="1">
+        <f>M21-L21</f>
         <v>-0.32751677852349004</v>
       </c>
-      <c r="O21" s="18">
+      <c r="Q21" s="18">
         <f t="shared" si="5"/>
-        <v>-1.3919463087248323</v>
-      </c>
-      <c r="P21" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.45185185185185195</v>
-      </c>
-      <c r="Q21" s="1">
-        <f t="shared" si="7"/>
-        <v>-1.2272189349112426</v>
+        <v>-0.77969924812030078</v>
       </c>
       <c r="R21" s="7" t="s">
         <v>43</v>
@@ -2478,49 +2435,47 @@
       <c r="E22">
         <v>3.42</v>
       </c>
-      <c r="F22" s="11">
+      <c r="F22" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="G22">
+        <v>1.19</v>
+      </c>
+      <c r="H22" s="11">
         <v>1.85</v>
       </c>
-      <c r="G22" s="1">
+      <c r="I22" s="1">
         <v>0.97799999999999998</v>
       </c>
-      <c r="H22" s="1">
+      <c r="J22" s="3">
         <v>0.80300000000000005</v>
       </c>
-      <c r="I22">
+      <c r="K22" s="4">
         <v>1.9E-2</v>
       </c>
-      <c r="J22" s="9">
+      <c r="L22" s="9">
         <f t="shared" si="0"/>
         <v>0.54093567251461994</v>
       </c>
-      <c r="K22" s="14">
+      <c r="M22" s="14">
         <f t="shared" si="1"/>
         <v>0.28596491228070176</v>
       </c>
-      <c r="L22" s="14">
+      <c r="N22" s="14">
         <f t="shared" si="2"/>
-        <v>0.23479532163742692</v>
-      </c>
-      <c r="M22" s="16">
+        <v>0.57357142857142862</v>
+      </c>
+      <c r="O22" s="16">
         <f t="shared" si="3"/>
-        <v>5.5555555555555558E-3</v>
-      </c>
-      <c r="N22" s="1">
+        <v>1.3571428571428571E-2</v>
+      </c>
+      <c r="P22" s="1">
         <f t="shared" si="4"/>
         <v>-0.25497076023391818</v>
       </c>
-      <c r="O22" s="1">
+      <c r="Q22" s="1">
         <f t="shared" si="5"/>
-        <v>-0.22923976608187135</v>
-      </c>
-      <c r="P22" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.47135135135135142</v>
-      </c>
-      <c r="Q22" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.97633872976338731</v>
+        <v>-0.56000000000000005</v>
       </c>
       <c r="R22" s="7" t="s">
         <v>27</v>
@@ -2542,49 +2497,47 @@
       <c r="E23">
         <v>0.33200000000000002</v>
       </c>
-      <c r="F23" s="10">
+      <c r="F23">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="G23">
+        <v>0.39300000000000002</v>
+      </c>
+      <c r="H23" s="10">
         <v>0.188</v>
       </c>
-      <c r="G23" s="1">
+      <c r="I23" s="1">
         <v>0.252</v>
       </c>
-      <c r="H23" s="1">
+      <c r="J23" s="1">
         <v>0.16600000000000001</v>
       </c>
-      <c r="I23">
+      <c r="K23">
         <v>0.248</v>
       </c>
-      <c r="J23" s="9">
+      <c r="L23" s="9">
         <f t="shared" si="0"/>
         <v>0.56626506024096379</v>
       </c>
-      <c r="K23" s="14">
+      <c r="M23" s="14">
         <f t="shared" si="1"/>
         <v>0.75903614457831325</v>
       </c>
-      <c r="L23" s="14">
+      <c r="N23" s="14">
         <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="M23" s="16">
+        <v>0.43229166666666669</v>
+      </c>
+      <c r="O23" s="16">
         <f t="shared" si="3"/>
-        <v>0.74698795180722888</v>
-      </c>
-      <c r="N23" s="1">
+        <v>0.64583333333333337</v>
+      </c>
+      <c r="P23" s="1">
         <f t="shared" si="4"/>
         <v>0.19277108433734946</v>
       </c>
-      <c r="O23" s="1">
+      <c r="Q23" s="1">
         <f t="shared" si="5"/>
-        <v>0.24698795180722888</v>
-      </c>
-      <c r="P23" s="10">
-        <f t="shared" si="6"/>
-        <v>0.34042553191489378</v>
-      </c>
-      <c r="Q23" s="1">
-        <f t="shared" si="7"/>
-        <v>0.49397590361445776</v>
+        <v>0.21354166666666669</v>
       </c>
       <c r="R23" s="7" t="s">
         <v>27</v>
@@ -2606,49 +2559,47 @@
       <c r="E24">
         <v>0.39700000000000002</v>
       </c>
-      <c r="F24" s="10">
+      <c r="F24">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="G24">
+        <v>0.376</v>
+      </c>
+      <c r="H24" s="10">
         <v>0.249</v>
       </c>
-      <c r="G24" s="1">
+      <c r="I24" s="1">
         <v>0.24</v>
       </c>
-      <c r="H24" s="1">
+      <c r="J24" s="1">
         <v>0.215</v>
       </c>
-      <c r="I24">
+      <c r="K24">
         <v>0.224</v>
       </c>
-      <c r="J24" s="9">
+      <c r="L24" s="9">
         <f t="shared" si="0"/>
         <v>0.62720403022670024</v>
       </c>
-      <c r="K24" s="14">
+      <c r="M24" s="14">
         <f t="shared" si="1"/>
         <v>0.60453400503778332</v>
       </c>
-      <c r="L24" s="14">
+      <c r="N24" s="14">
         <f t="shared" si="2"/>
-        <v>0.54156171284634758</v>
-      </c>
-      <c r="M24" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="O24" s="16">
         <f t="shared" si="3"/>
-        <v>0.5642317380352645</v>
-      </c>
-      <c r="N24" s="1">
+        <v>0.65116279069767447</v>
+      </c>
+      <c r="P24" s="1">
         <f t="shared" si="4"/>
         <v>-2.267002518891692E-2</v>
       </c>
-      <c r="O24" s="1">
+      <c r="Q24" s="1">
         <f t="shared" si="5"/>
-        <v>2.267002518891692E-2</v>
-      </c>
-      <c r="P24" s="10">
-        <f t="shared" si="6"/>
-        <v>-3.614457831325308E-2</v>
-      </c>
-      <c r="Q24" s="1">
-        <f t="shared" si="7"/>
-        <v>4.1860465116279152E-2</v>
+        <v>2.6162790697674465E-2</v>
       </c>
       <c r="R24" s="7" t="s">
         <v>27</v>
@@ -2670,49 +2621,47 @@
       <c r="E25">
         <v>0.46400000000000002</v>
       </c>
-      <c r="F25" s="10">
+      <c r="F25">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="G25">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="H25" s="10">
         <v>0.25800000000000001</v>
       </c>
-      <c r="G25" s="1">
+      <c r="I25" s="1">
         <v>4.4999999999999998E-2</v>
       </c>
-      <c r="H25" s="1">
+      <c r="J25" s="1">
         <v>0.28899999999999998</v>
       </c>
-      <c r="I25">
+      <c r="K25">
         <v>-4.9000000000000002E-2</v>
       </c>
-      <c r="J25" s="9">
+      <c r="L25" s="9">
         <f t="shared" si="0"/>
         <v>0.55603448275862066</v>
       </c>
-      <c r="K25" s="14">
+      <c r="M25" s="14">
         <f t="shared" si="1"/>
         <v>9.6982758620689641E-2</v>
       </c>
-      <c r="L25" s="14">
+      <c r="N25" s="14">
         <f t="shared" si="2"/>
-        <v>0.62284482758620685</v>
-      </c>
-      <c r="M25" s="16">
+        <v>0.63656387665198233</v>
+      </c>
+      <c r="O25" s="16">
         <f t="shared" si="3"/>
-        <v>-0.10560344827586207</v>
-      </c>
-      <c r="N25" s="1">
+        <v>-0.10792951541850221</v>
+      </c>
+      <c r="P25" s="1">
         <f t="shared" si="4"/>
         <v>-0.45905172413793105</v>
       </c>
-      <c r="O25" s="1">
+      <c r="Q25" s="1">
         <f t="shared" si="5"/>
-        <v>-0.72844827586206895</v>
-      </c>
-      <c r="P25" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.82558139534883723</v>
-      </c>
-      <c r="Q25" s="1">
-        <f t="shared" si="7"/>
-        <v>-1.1695501730103808</v>
+        <v>-0.74449339207048459</v>
       </c>
       <c r="R25" s="7" t="s">
         <v>43</v>
@@ -2734,49 +2683,47 @@
       <c r="E26">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F26" s="10">
+      <c r="F26">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="G26">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="H26" s="10">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="G26" s="1">
+      <c r="I26" s="1">
         <v>-0.192</v>
       </c>
-      <c r="H26" s="1">
+      <c r="J26" s="1">
         <v>5.7000000000000002E-2</v>
       </c>
-      <c r="I26">
+      <c r="K26">
         <v>-5.8999999999999997E-2</v>
       </c>
-      <c r="J26" s="9">
+      <c r="L26" s="9">
         <f t="shared" si="0"/>
         <v>0.53237410071942437</v>
       </c>
-      <c r="K26" s="14">
-        <f>G26/$E26</f>
+      <c r="M26" s="14">
+        <f t="shared" si="1"/>
         <v>-1.3812949640287768</v>
       </c>
-      <c r="L26" s="14">
+      <c r="N26" s="14">
         <f t="shared" si="2"/>
-        <v>0.41007194244604317</v>
-      </c>
-      <c r="M26" s="16">
+        <v>0.39583333333333337</v>
+      </c>
+      <c r="O26" s="16">
         <f t="shared" si="3"/>
-        <v>-0.42446043165467617</v>
-      </c>
-      <c r="N26" s="3">
-        <f>K26-J26</f>
+        <v>-0.40972222222222221</v>
+      </c>
+      <c r="P26" s="3">
+        <f>M26-L26</f>
         <v>-1.9136690647482011</v>
       </c>
-      <c r="O26" s="1">
-        <f>M26-L26</f>
-        <v>-0.83453237410071934</v>
-      </c>
-      <c r="P26" s="10">
-        <f>(K26-J26)/ABS(J26)</f>
-        <v>-3.5945945945945947</v>
-      </c>
       <c r="Q26" s="1">
-        <f t="shared" si="7"/>
-        <v>-2.0350877192982453</v>
+        <f>O26-N26</f>
+        <v>-0.80555555555555558</v>
       </c>
       <c r="R26" s="7" t="s">
         <v>43</v>
@@ -2798,49 +2745,47 @@
       <c r="E27">
         <v>0.29899999999999999</v>
       </c>
-      <c r="F27" s="10">
+      <c r="F27" s="1">
+        <v>0.34</v>
+      </c>
+      <c r="G27">
+        <v>-2.9000000000000001E-2</v>
+      </c>
+      <c r="H27" s="10">
         <v>0.16700000000000001</v>
       </c>
-      <c r="G27" s="1">
+      <c r="I27" s="1">
         <v>-0.186</v>
       </c>
-      <c r="H27" s="1">
+      <c r="J27" s="1">
         <v>0.19900000000000001</v>
       </c>
-      <c r="I27">
+      <c r="K27">
         <v>-7.9000000000000001E-2</v>
       </c>
-      <c r="J27" s="9">
+      <c r="L27" s="9">
         <f t="shared" si="0"/>
         <v>0.55852842809364556</v>
       </c>
-      <c r="K27" s="14">
+      <c r="M27" s="14">
         <f t="shared" si="1"/>
         <v>-0.62207357859531776</v>
       </c>
-      <c r="L27" s="14">
+      <c r="N27" s="14">
         <f t="shared" si="2"/>
-        <v>0.66555183946488305</v>
-      </c>
-      <c r="M27" s="16">
+        <v>0.58529411764705885</v>
+      </c>
+      <c r="O27" s="16">
         <f t="shared" si="3"/>
-        <v>-0.26421404682274247</v>
-      </c>
-      <c r="N27" s="1">
+        <v>-0.23235294117647057</v>
+      </c>
+      <c r="P27" s="1">
         <f t="shared" si="4"/>
         <v>-1.1806020066889633</v>
       </c>
-      <c r="O27" s="1">
+      <c r="Q27" s="1">
         <f t="shared" si="5"/>
-        <v>-0.92976588628762546</v>
-      </c>
-      <c r="P27" s="10">
-        <f t="shared" si="6"/>
-        <v>-2.1137724550898205</v>
-      </c>
-      <c r="Q27" s="1">
-        <f t="shared" si="7"/>
-        <v>-1.3969849246231154</v>
+        <v>-0.81764705882352939</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>43</v>
@@ -2862,49 +2807,47 @@
       <c r="E28">
         <v>0.35699999999999998</v>
       </c>
-      <c r="F28" s="10">
+      <c r="F28" s="1">
+        <v>0.48</v>
+      </c>
+      <c r="G28">
+        <v>0.38800000000000001</v>
+      </c>
+      <c r="H28" s="10">
         <v>0.21199999999999999</v>
       </c>
-      <c r="G28" s="1">
+      <c r="I28" s="1">
         <v>0.11799999999999999</v>
       </c>
-      <c r="H28" s="1">
+      <c r="J28" s="1">
         <v>0.27200000000000002</v>
       </c>
-      <c r="I28" s="1">
+      <c r="K28" s="1">
         <v>9.2999999999999999E-2</v>
       </c>
-      <c r="J28" s="9">
+      <c r="L28" s="9">
         <f t="shared" si="0"/>
         <v>0.5938375350140056</v>
       </c>
-      <c r="K28" s="14">
+      <c r="M28" s="14">
         <f t="shared" si="1"/>
         <v>0.33053221288515405</v>
       </c>
-      <c r="L28" s="14">
+      <c r="N28" s="14">
         <f t="shared" si="2"/>
-        <v>0.76190476190476197</v>
-      </c>
-      <c r="M28" s="16">
+        <v>0.56666666666666676</v>
+      </c>
+      <c r="O28" s="16">
         <f t="shared" si="3"/>
-        <v>0.26050420168067229</v>
-      </c>
-      <c r="N28" s="1">
+        <v>0.19375000000000001</v>
+      </c>
+      <c r="P28" s="1">
         <f t="shared" si="4"/>
         <v>-0.26330532212885155</v>
       </c>
-      <c r="O28" s="1">
+      <c r="Q28" s="1">
         <f t="shared" si="5"/>
-        <v>-0.50140056022408963</v>
-      </c>
-      <c r="P28" s="10">
-        <f t="shared" si="6"/>
-        <v>-0.44339622641509435</v>
-      </c>
-      <c r="Q28" s="1">
-        <f t="shared" si="7"/>
-        <v>-0.65808823529411753</v>
+        <v>-0.37291666666666679</v>
       </c>
       <c r="R28" s="7" t="s">
         <v>27</v>
@@ -2912,8 +2855,5 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <ignoredErrors>
-    <ignoredError sqref="P26" formula="1"/>
-  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixed errors in quantifying life history traits from TPCs and DDE model
</commit_message>
<xml_diff>
--- a/Model results Tave.xlsx
+++ b/Model results Tave.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B70F32-367C-5B49-8A4B-2F9992BE2967}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81323491-6865-3041-9322-6A7D6F10FC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6200" yWindow="500" windowWidth="22560" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1880" yWindow="500" windowWidth="26880" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Model results" sheetId="1" r:id="rId1"/>
@@ -41,9 +41,6 @@
     <t>Habitat</t>
   </si>
   <si>
-    <t>subfamily</t>
-  </si>
-  <si>
     <t>r.TPC.h</t>
   </si>
   <si>
@@ -189,6 +186,9 @@
   </si>
   <si>
     <t>rMax.model.h</t>
+  </si>
+  <si>
+    <t>Subfamily</t>
   </si>
 </sst>
 </file>
@@ -346,7 +346,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -524,6 +524,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -736,27 +742,22 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
     <xf numFmtId="164" fontId="19" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1115,8 +1116,8 @@
   <dimension ref="A1:R28"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="G1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="N11" sqref="N11"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1124,1726 +1125,1728 @@
     <col min="1" max="1" width="44.83203125" customWidth="1"/>
     <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="13.5" customWidth="1"/>
-    <col min="7" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="35.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>51</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="H1" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="G1" s="12" t="s">
-        <v>51</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>46</v>
-      </c>
-      <c r="I1" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="K1" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="L1" s="13" t="s">
+      <c r="M1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="N1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="12" t="s">
+      <c r="O1" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="15" t="s">
+      <c r="P1" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="Q1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="R1" s="7" t="s">
         <v>7</v>
-      </c>
-      <c r="P1" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="Q1" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2">
         <v>6.45</v>
       </c>
       <c r="C2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" t="s">
         <v>10</v>
-      </c>
-      <c r="D2" t="s">
-        <v>11</v>
       </c>
       <c r="E2">
         <v>0.13400000000000001</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="12">
         <v>0.127</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="12">
         <v>0.108</v>
       </c>
-      <c r="H2" s="8">
-        <v>0.127</v>
-      </c>
-      <c r="I2" s="6">
-        <v>8.3000000000000004E-2</v>
-      </c>
-      <c r="J2" s="6">
-        <v>0.12</v>
-      </c>
-      <c r="K2" s="5">
-        <v>7.5999999999999998E-2</v>
-      </c>
-      <c r="L2" s="9">
+      <c r="H2" s="1">
+        <v>0.12731838000000001</v>
+      </c>
+      <c r="I2" s="1">
+        <v>8.2553520000000005E-2</v>
+      </c>
+      <c r="J2" s="1">
+        <v>0.12038422</v>
+      </c>
+      <c r="K2" s="1">
+        <v>7.6048909999999997E-2</v>
+      </c>
+      <c r="L2" s="5">
         <f>H2/$E2</f>
-        <v>0.94776119402985071</v>
-      </c>
-      <c r="M2" s="14">
+        <v>0.95013716417910443</v>
+      </c>
+      <c r="M2" s="8">
         <f>I2/$E2</f>
-        <v>0.61940298507462688</v>
-      </c>
-      <c r="N2" s="14">
+        <v>0.6160710447761194</v>
+      </c>
+      <c r="N2" s="8">
         <f>J2/$E2</f>
-        <v>0.89552238805970141</v>
-      </c>
-      <c r="O2" s="16">
+        <v>0.89838970149253727</v>
+      </c>
+      <c r="O2" s="10">
         <f>K2/$E2</f>
-        <v>0.56716417910447758</v>
+        <v>0.56752917910447753</v>
       </c>
       <c r="P2" s="1">
         <f>M2-L2</f>
-        <v>-0.32835820895522383</v>
+        <v>-0.33406611940298503</v>
       </c>
       <c r="Q2" s="1">
         <f>O2-N2</f>
-        <v>-0.32835820895522383</v>
-      </c>
-      <c r="R2" s="7"/>
+        <v>-0.33086052238805974</v>
+      </c>
+      <c r="R2" s="4"/>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B3">
         <v>6.45</v>
       </c>
       <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>10</v>
-      </c>
-      <c r="D3" t="s">
-        <v>11</v>
       </c>
       <c r="E3">
         <v>0.154</v>
       </c>
-      <c r="F3">
+      <c r="F3" s="12">
         <v>0.13200000000000001</v>
       </c>
-      <c r="G3">
+      <c r="G3" s="12">
         <v>0.157</v>
       </c>
-      <c r="H3" s="9">
-        <v>0.125</v>
-      </c>
-      <c r="I3" s="5">
-        <v>0.152</v>
-      </c>
-      <c r="J3" s="5">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="K3" s="5">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="L3" s="9">
+      <c r="H3" s="1">
+        <v>0.12525969000000001</v>
+      </c>
+      <c r="I3" s="1">
+        <v>0.15241109999999999</v>
+      </c>
+      <c r="J3" s="1">
+        <v>0.1159646</v>
+      </c>
+      <c r="K3" s="1">
+        <v>0.14839018000000001</v>
+      </c>
+      <c r="L3" s="5">
         <f t="shared" ref="L3:L28" si="0">H3/$E3</f>
-        <v>0.81168831168831168</v>
-      </c>
-      <c r="M3" s="14">
+        <v>0.81337461038961045</v>
+      </c>
+      <c r="M3" s="8">
         <f t="shared" ref="M3:M28" si="1">I3/$E3</f>
-        <v>0.98701298701298701</v>
-      </c>
-      <c r="N3" s="14">
+        <v>0.98968246753246747</v>
+      </c>
+      <c r="N3" s="8">
         <f t="shared" ref="N3:N28" si="2">J3/$E3</f>
-        <v>0.75324675324675328</v>
-      </c>
-      <c r="O3" s="16">
+        <v>0.75301688311688308</v>
+      </c>
+      <c r="O3" s="10">
         <f t="shared" ref="O3:O28" si="3">K3/$E3</f>
-        <v>0.96103896103896103</v>
+        <v>0.96357259740259749</v>
       </c>
       <c r="P3" s="1">
         <f t="shared" ref="P3:P28" si="4">M3-L3</f>
-        <v>0.17532467532467533</v>
+        <v>0.17630785714285702</v>
       </c>
       <c r="Q3" s="1">
         <f t="shared" ref="Q3:Q28" si="5">O3-N3</f>
-        <v>0.20779220779220775</v>
-      </c>
-      <c r="R3" s="7"/>
+        <v>0.2105557142857144</v>
+      </c>
+      <c r="R3" s="4"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B4">
         <v>7.45</v>
       </c>
       <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
-      </c>
-      <c r="D4" t="s">
-        <v>11</v>
       </c>
       <c r="E4">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="12">
         <v>0.182</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="12">
         <v>0.19800000000000001</v>
       </c>
-      <c r="H4" s="9">
-        <v>7.9000000000000001E-2</v>
-      </c>
-      <c r="I4" s="6">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="J4" s="5">
-        <v>0.159</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0.19400000000000001</v>
-      </c>
-      <c r="L4" s="9">
+      <c r="H4" s="1">
+        <v>7.8510609999999995E-2</v>
+      </c>
+      <c r="I4" s="1">
+        <v>8.6862099999999998E-2</v>
+      </c>
+      <c r="J4" s="1">
+        <v>0.15893209</v>
+      </c>
+      <c r="K4" s="1">
+        <v>0.19348343000000001</v>
+      </c>
+      <c r="L4" s="5">
         <f t="shared" si="0"/>
-        <v>0.89772727272727282</v>
-      </c>
-      <c r="M4" s="14">
+        <v>0.89216602272727275</v>
+      </c>
+      <c r="M4" s="8">
         <f t="shared" si="1"/>
-        <v>0.98863636363636365</v>
-      </c>
-      <c r="N4" s="14">
+        <v>0.9870693181818182</v>
+      </c>
+      <c r="N4" s="8">
         <f t="shared" si="2"/>
-        <v>1.8068181818181819</v>
-      </c>
-      <c r="O4" s="16">
+        <v>1.8060464772727274</v>
+      </c>
+      <c r="O4" s="10">
         <f t="shared" si="3"/>
-        <v>2.2045454545454546</v>
+        <v>2.1986753409090913</v>
       </c>
       <c r="P4" s="1">
         <f t="shared" si="4"/>
-        <v>9.0909090909090828E-2</v>
+        <v>9.4903295454545455E-2</v>
       </c>
       <c r="Q4" s="1">
         <f t="shared" si="5"/>
-        <v>0.39772727272727271</v>
-      </c>
-      <c r="R4" s="7"/>
+        <v>0.39262886363636396</v>
+      </c>
+      <c r="R4" s="4"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5">
         <v>12.38</v>
       </c>
       <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
         <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>11</v>
       </c>
       <c r="E5">
         <v>8.7999999999999995E-2</v>
       </c>
-      <c r="F5">
+      <c r="F5" s="12">
         <v>0.104</v>
       </c>
-      <c r="G5">
+      <c r="G5" s="12">
         <v>9.0999999999999998E-2</v>
       </c>
-      <c r="H5" s="8">
-        <v>8.1000000000000003E-2</v>
-      </c>
-      <c r="I5" s="6">
-        <v>8.2000000000000003E-2</v>
-      </c>
-      <c r="J5" s="6">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="K5" s="6">
-        <v>4.9000000000000002E-2</v>
-      </c>
-      <c r="L5" s="9">
+      <c r="H5" s="1">
+        <v>8.1424479999999994E-2</v>
+      </c>
+      <c r="I5" s="1">
+        <v>8.2125939999999995E-2</v>
+      </c>
+      <c r="J5" s="1">
+        <v>9.0818270000000006E-2</v>
+      </c>
+      <c r="K5" s="1">
+        <v>4.9424460000000003E-2</v>
+      </c>
+      <c r="L5" s="5">
         <f t="shared" si="0"/>
-        <v>0.92045454545454553</v>
-      </c>
-      <c r="M5" s="14">
+        <v>0.92527818181818178</v>
+      </c>
+      <c r="M5" s="8">
         <f t="shared" si="1"/>
-        <v>0.93181818181818188</v>
-      </c>
-      <c r="N5" s="14">
+        <v>0.93324931818181822</v>
+      </c>
+      <c r="N5" s="8">
         <f t="shared" si="2"/>
-        <v>1.0340909090909092</v>
-      </c>
-      <c r="O5" s="16">
+        <v>1.0320257954545455</v>
+      </c>
+      <c r="O5" s="10">
         <f t="shared" si="3"/>
-        <v>0.55681818181818188</v>
+        <v>0.56164159090909094</v>
       </c>
       <c r="P5" s="1">
         <f t="shared" si="4"/>
-        <v>1.1363636363636354E-2</v>
+        <v>7.9711363636364441E-3</v>
       </c>
       <c r="Q5" s="1">
         <f t="shared" si="5"/>
-        <v>-0.47727272727272729</v>
-      </c>
-      <c r="R5" s="7"/>
+        <v>-0.4703842045454546</v>
+      </c>
+      <c r="R5" s="4"/>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6">
         <v>33.33</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="12">
         <v>0.13800000000000001</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="12">
         <v>0.106</v>
       </c>
-      <c r="H6" s="9">
-        <v>0.104</v>
-      </c>
-      <c r="I6" s="6">
-        <v>0.109</v>
-      </c>
-      <c r="J6" s="5">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="K6" s="6">
-        <v>0.10100000000000001</v>
-      </c>
-      <c r="L6" s="9">
+      <c r="H6" s="1">
+        <v>0.10430294</v>
+      </c>
+      <c r="I6" s="1">
+        <v>0.10871624000000001</v>
+      </c>
+      <c r="J6" s="1">
+        <v>0.1221749</v>
+      </c>
+      <c r="K6" s="1">
+        <v>0.10082707</v>
+      </c>
+      <c r="L6" s="5">
         <f t="shared" si="0"/>
-        <v>0.63030303030303025</v>
-      </c>
-      <c r="M6" s="14">
+        <v>0.6321390303030302</v>
+      </c>
+      <c r="M6" s="8">
         <f t="shared" si="1"/>
-        <v>0.66060606060606053</v>
-      </c>
-      <c r="N6" s="14">
+        <v>0.65888630303030304</v>
+      </c>
+      <c r="N6" s="8">
         <f t="shared" si="2"/>
-        <v>0.61818181818181817</v>
-      </c>
-      <c r="O6" s="16">
+        <v>0.74045393939393933</v>
+      </c>
+      <c r="O6" s="10">
         <f t="shared" si="3"/>
-        <v>0.61212121212121218</v>
+        <v>0.61107315151515151</v>
       </c>
       <c r="P6" s="1">
         <f t="shared" si="4"/>
-        <v>3.0303030303030276E-2</v>
+        <v>2.6747272727272842E-2</v>
       </c>
       <c r="Q6" s="1">
         <f t="shared" si="5"/>
-        <v>-6.0606060606059886E-3</v>
-      </c>
-      <c r="R6" s="7" t="s">
-        <v>27</v>
+        <v>-0.12938078787878782</v>
+      </c>
+      <c r="R6" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B7">
         <v>33.33</v>
       </c>
       <c r="C7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E7">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="12">
         <v>0.155</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="12">
         <v>9.6000000000000002E-2</v>
       </c>
-      <c r="H7" s="9">
-        <v>5.1999999999999998E-2</v>
-      </c>
-      <c r="I7" s="6">
-        <v>6.3E-2</v>
-      </c>
-      <c r="J7" s="5">
-        <v>9.0999999999999998E-2</v>
-      </c>
-      <c r="K7" s="6">
-        <v>8.5000000000000006E-2</v>
-      </c>
-      <c r="L7" s="9">
+      <c r="H7" s="1">
+        <v>5.2348279999999997E-2</v>
+      </c>
+      <c r="I7" s="1">
+        <v>6.275936E-2</v>
+      </c>
+      <c r="J7" s="1">
+        <v>0.11939899</v>
+      </c>
+      <c r="K7" s="1">
+        <v>8.4682789999999994E-2</v>
+      </c>
+      <c r="L7" s="5">
         <f t="shared" si="0"/>
-        <v>0.62650602409638545</v>
-      </c>
-      <c r="M7" s="14">
+        <v>0.63070216867469875</v>
+      </c>
+      <c r="M7" s="8">
         <f t="shared" si="1"/>
-        <v>0.75903614457831325</v>
-      </c>
-      <c r="N7" s="14">
+        <v>0.75613686746987951</v>
+      </c>
+      <c r="N7" s="8">
         <f t="shared" si="2"/>
-        <v>1.0963855421686746</v>
-      </c>
-      <c r="O7" s="16">
+        <v>1.4385420481927709</v>
+      </c>
+      <c r="O7" s="10">
         <f t="shared" si="3"/>
-        <v>1.0240963855421688</v>
+        <v>1.020274578313253</v>
       </c>
       <c r="P7" s="1">
         <f t="shared" si="4"/>
-        <v>0.1325301204819278</v>
+        <v>0.12543469879518077</v>
       </c>
       <c r="Q7" s="1">
         <f t="shared" si="5"/>
-        <v>-7.2289156626505813E-2</v>
-      </c>
-      <c r="R7" s="7" t="s">
-        <v>27</v>
+        <v>-0.41826746987951791</v>
+      </c>
+      <c r="R7" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8">
         <v>39.880000000000003</v>
       </c>
       <c r="C8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E8">
         <v>0.16500000000000001</v>
       </c>
-      <c r="F8">
+      <c r="F8" s="12">
         <v>0.219</v>
       </c>
-      <c r="G8">
+      <c r="G8" s="12">
         <v>0.29599999999999999</v>
       </c>
-      <c r="H8" s="8">
-        <v>0.105</v>
-      </c>
-      <c r="I8" s="6">
-        <v>0.11600000000000001</v>
-      </c>
-      <c r="J8" s="5">
-        <v>0.16500000000000001</v>
-      </c>
-      <c r="K8" s="5">
-        <v>0.22700000000000001</v>
-      </c>
-      <c r="L8" s="9">
+      <c r="H8" s="1">
+        <v>0.10529814999999999</v>
+      </c>
+      <c r="I8" s="1">
+        <v>0.11626292000000001</v>
+      </c>
+      <c r="J8" s="1">
+        <v>0.18692663000000001</v>
+      </c>
+      <c r="K8" s="1">
+        <v>0.24501068000000001</v>
+      </c>
+      <c r="L8" s="5">
         <f t="shared" si="0"/>
-        <v>0.63636363636363635</v>
-      </c>
-      <c r="M8" s="14">
+        <v>0.63817060606060594</v>
+      </c>
+      <c r="M8" s="8">
         <f t="shared" si="1"/>
-        <v>0.70303030303030301</v>
-      </c>
-      <c r="N8" s="14">
+        <v>0.70462375757575757</v>
+      </c>
+      <c r="N8" s="8">
         <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="O8" s="16">
+        <v>1.1328886666666667</v>
+      </c>
+      <c r="O8" s="10">
         <f t="shared" si="3"/>
-        <v>1.3757575757575757</v>
+        <v>1.4849132121212121</v>
       </c>
       <c r="P8" s="1">
         <f t="shared" si="4"/>
-        <v>6.6666666666666652E-2</v>
+        <v>6.6453151515151632E-2</v>
       </c>
       <c r="Q8" s="1">
         <f t="shared" si="5"/>
-        <v>0.37575757575757573</v>
-      </c>
-      <c r="R8" s="7" t="s">
-        <v>27</v>
+        <v>0.35202454545454542</v>
+      </c>
+      <c r="R8" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9">
         <v>35.53</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E9">
         <v>8.3000000000000004E-2</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="12">
         <v>0.17799999999999999</v>
       </c>
-      <c r="G9" s="1">
+      <c r="G9" s="13">
         <v>0.16</v>
       </c>
-      <c r="H9" s="9">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="I9" s="6">
-        <v>5.3999999999999999E-2</v>
-      </c>
-      <c r="J9" s="5">
-        <v>0.107</v>
-      </c>
-      <c r="K9" s="5">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="L9" s="9">
+      <c r="H9" s="1">
+        <v>5.3774000000000002E-2</v>
+      </c>
+      <c r="I9" s="1">
+        <v>5.444036E-2</v>
+      </c>
+      <c r="J9" s="1">
+        <v>0.13774874000000001</v>
+      </c>
+      <c r="K9" s="1">
+        <v>0.11792382999999999</v>
+      </c>
+      <c r="L9" s="5">
         <f t="shared" si="0"/>
-        <v>0.6506024096385542</v>
-      </c>
-      <c r="M9" s="14">
+        <v>0.64787951807228916</v>
+      </c>
+      <c r="M9" s="8">
         <f t="shared" si="1"/>
-        <v>0.6506024096385542</v>
-      </c>
-      <c r="N9" s="14">
+        <v>0.65590795180722883</v>
+      </c>
+      <c r="N9" s="8">
         <f t="shared" si="2"/>
-        <v>1.2891566265060239</v>
-      </c>
-      <c r="O9" s="16">
+        <v>1.6596233734939758</v>
+      </c>
+      <c r="O9" s="10">
         <f t="shared" si="3"/>
-        <v>1.1204819277108433</v>
+        <v>1.4207690361445782</v>
       </c>
       <c r="P9" s="1">
         <f t="shared" si="4"/>
-        <v>0</v>
+        <v>8.0284337349396662E-3</v>
       </c>
       <c r="Q9" s="1">
         <f t="shared" si="5"/>
-        <v>-0.1686746987951806</v>
-      </c>
-      <c r="R9" s="7" t="s">
-        <v>27</v>
+        <v>-0.23885433734939765</v>
+      </c>
+      <c r="R9" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10">
         <v>21.23</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E10">
         <v>0.246</v>
       </c>
-      <c r="F10" s="1">
+      <c r="F10" s="13">
         <v>0.69</v>
       </c>
-      <c r="G10">
+      <c r="G10" s="12">
         <v>0.67600000000000005</v>
       </c>
-      <c r="H10" s="9">
-        <v>0.23400000000000001</v>
-      </c>
-      <c r="I10" s="6">
-        <v>0.215</v>
-      </c>
-      <c r="J10" s="6">
-        <v>0.66</v>
-      </c>
-      <c r="K10" s="5">
-        <v>0.46400000000000002</v>
-      </c>
-      <c r="L10" s="9">
+      <c r="H10" s="1">
+        <v>0.18755553</v>
+      </c>
+      <c r="I10" s="1">
+        <v>8.9563599999999993E-2</v>
+      </c>
+      <c r="J10" s="1">
+        <v>0.65640953999999996</v>
+      </c>
+      <c r="K10" s="1">
+        <v>0.59114586000000002</v>
+      </c>
+      <c r="L10" s="5">
         <f t="shared" si="0"/>
-        <v>0.95121951219512202</v>
-      </c>
-      <c r="M10" s="14">
+        <v>0.76242085365853662</v>
+      </c>
+      <c r="M10" s="8">
         <f t="shared" si="1"/>
-        <v>0.87398373983739841</v>
-      </c>
-      <c r="N10" s="14">
+        <v>0.36407967479674797</v>
+      </c>
+      <c r="N10" s="8">
         <f t="shared" si="2"/>
-        <v>2.6829268292682928</v>
-      </c>
-      <c r="O10" s="16">
+        <v>2.668331463414634</v>
+      </c>
+      <c r="O10" s="10">
         <f t="shared" si="3"/>
-        <v>1.8861788617886179</v>
+        <v>2.4030319512195124</v>
       </c>
       <c r="P10" s="1">
         <f t="shared" si="4"/>
-        <v>-7.7235772357723609E-2</v>
+        <v>-0.39834117886178866</v>
       </c>
       <c r="Q10" s="1">
         <f t="shared" si="5"/>
-        <v>-0.79674796747967491</v>
-      </c>
-      <c r="R10" s="7"/>
+        <v>-0.2652995121951216</v>
+      </c>
+      <c r="R10" s="4"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B11">
         <v>21.23</v>
       </c>
       <c r="C11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E11">
         <v>0.25700000000000001</v>
       </c>
-      <c r="F11">
+      <c r="F11" s="12">
         <v>0.72199999999999998</v>
       </c>
-      <c r="G11">
+      <c r="G11" s="12">
         <v>0.69499999999999995</v>
       </c>
-      <c r="H11" s="9">
-        <v>0.24099999999999999</v>
-      </c>
-      <c r="I11" s="6">
-        <v>0.19600000000000001</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0.68400000000000005</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0.379</v>
-      </c>
-      <c r="L11" s="9">
+      <c r="H11" s="1">
+        <v>0.14664637999999999</v>
+      </c>
+      <c r="I11" s="1">
+        <v>-2.6436000000000001E-2</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0.68685766999999998</v>
+      </c>
+      <c r="K11" s="1">
+        <v>0.55110091000000005</v>
+      </c>
+      <c r="L11" s="5">
         <f t="shared" si="0"/>
-        <v>0.9377431906614786</v>
-      </c>
-      <c r="M11" s="14">
+        <v>0.5706084824902723</v>
+      </c>
+      <c r="M11" s="8">
         <f t="shared" si="1"/>
-        <v>0.76264591439688723</v>
-      </c>
-      <c r="N11" s="14">
+        <v>-0.10286381322957198</v>
+      </c>
+      <c r="N11" s="8">
         <f t="shared" si="2"/>
-        <v>2.6614785992217902</v>
-      </c>
-      <c r="O11" s="16">
+        <v>2.6725979377431903</v>
+      </c>
+      <c r="O11" s="10">
         <f t="shared" si="3"/>
-        <v>1.4747081712062255</v>
+        <v>2.1443615175097279</v>
       </c>
       <c r="P11" s="1">
         <f t="shared" si="4"/>
-        <v>-0.17509727626459137</v>
+        <v>-0.67347229571984424</v>
       </c>
       <c r="Q11" s="1">
         <f t="shared" si="5"/>
-        <v>-1.1867704280155646</v>
-      </c>
-      <c r="R11" s="7"/>
+        <v>-0.5282364202334624</v>
+      </c>
+      <c r="R11" s="4"/>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B12">
         <v>21.23</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E12">
         <v>0.249</v>
       </c>
-      <c r="F12">
+      <c r="F12" s="12">
         <v>0.78100000000000003</v>
       </c>
-      <c r="G12">
+      <c r="G12" s="12">
         <v>0.77400000000000002</v>
       </c>
-      <c r="H12" s="8">
-        <v>0.23100000000000001</v>
-      </c>
-      <c r="I12" s="6">
-        <v>0.19700000000000001</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0.73599999999999999</v>
-      </c>
-      <c r="K12" s="5">
-        <v>0.54700000000000004</v>
-      </c>
-      <c r="L12" s="9">
+      <c r="H12" s="1">
+        <v>0.23084498000000001</v>
+      </c>
+      <c r="I12" s="1">
+        <v>0.19656571</v>
+      </c>
+      <c r="J12" s="1">
+        <v>0.73036701000000004</v>
+      </c>
+      <c r="K12" s="1">
+        <v>0.55772034000000004</v>
+      </c>
+      <c r="L12" s="5">
         <f t="shared" si="0"/>
-        <v>0.92771084337349408</v>
-      </c>
-      <c r="M12" s="14">
+        <v>0.92708827309236952</v>
+      </c>
+      <c r="M12" s="8">
         <f t="shared" si="1"/>
-        <v>0.79116465863453822</v>
-      </c>
-      <c r="N12" s="14">
+        <v>0.78942052208835345</v>
+      </c>
+      <c r="N12" s="8">
         <f t="shared" si="2"/>
-        <v>2.9558232931726907</v>
-      </c>
-      <c r="O12" s="16">
+        <v>2.933200843373494</v>
+      </c>
+      <c r="O12" s="10">
         <f t="shared" si="3"/>
-        <v>2.1967871485943777</v>
+        <v>2.2398407228915662</v>
       </c>
       <c r="P12" s="1">
         <f t="shared" si="4"/>
-        <v>-0.13654618473895586</v>
+        <v>-0.13766775100401607</v>
       </c>
       <c r="Q12" s="1">
         <f t="shared" si="5"/>
-        <v>-0.75903614457831292</v>
-      </c>
-      <c r="R12" s="7"/>
+        <v>-0.69336012048192774</v>
+      </c>
+      <c r="R12" s="4"/>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B13">
         <v>38.380000000000003</v>
       </c>
       <c r="C13" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D13" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E13" s="1">
         <v>0.1</v>
       </c>
-      <c r="F13" s="1">
+      <c r="F13" s="13">
         <v>0.14000000000000001</v>
       </c>
-      <c r="G13" s="1">
+      <c r="G13" s="13">
         <v>0.192</v>
       </c>
-      <c r="H13" s="10">
-        <v>5.8999999999999997E-2</v>
+      <c r="H13" s="1">
+        <v>6.9977120000000004E-2</v>
       </c>
       <c r="I13" s="1">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="J13" s="3">
-        <v>8.4000000000000005E-2</v>
-      </c>
-      <c r="K13" s="4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="L13" s="9">
+        <v>9.1284859999999995E-2</v>
+      </c>
+      <c r="J13" s="1">
+        <v>8.4228399999999995E-2</v>
+      </c>
+      <c r="K13" s="1">
+        <v>5.8748309999999998E-2</v>
+      </c>
+      <c r="L13" s="5">
         <f t="shared" si="0"/>
-        <v>0.59</v>
-      </c>
-      <c r="M13" s="14">
+        <v>0.69977120000000004</v>
+      </c>
+      <c r="M13" s="8">
         <f t="shared" si="1"/>
-        <v>0.34</v>
-      </c>
-      <c r="N13" s="14">
+        <v>0.9128485999999999</v>
+      </c>
+      <c r="N13" s="8">
         <f t="shared" si="2"/>
-        <v>0.84</v>
-      </c>
-      <c r="O13" s="16">
+        <v>0.84228399999999992</v>
+      </c>
+      <c r="O13" s="10">
         <f t="shared" si="3"/>
-        <v>0.74999999999999989</v>
+        <v>0.58748309999999992</v>
       </c>
       <c r="P13" s="1">
         <f t="shared" si="4"/>
-        <v>-0.24999999999999994</v>
+        <v>0.21307739999999986</v>
       </c>
       <c r="Q13" s="1">
         <f t="shared" si="5"/>
-        <v>-9.000000000000008E-2</v>
-      </c>
-      <c r="R13" s="7" t="s">
-        <v>27</v>
+        <v>-0.2548009</v>
+      </c>
+      <c r="R13" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14">
         <v>38.380000000000003</v>
       </c>
       <c r="C14" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D14" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E14">
         <v>0.104</v>
       </c>
-      <c r="F14">
+      <c r="F14" s="12">
         <v>0.14799999999999999</v>
       </c>
-      <c r="G14">
+      <c r="G14" s="12">
         <v>0.19900000000000001</v>
       </c>
-      <c r="H14" s="10">
-        <v>5.8999999999999997E-2</v>
+      <c r="H14" s="1">
+        <v>6.8920449999999994E-2</v>
       </c>
       <c r="I14" s="1">
-        <v>0</v>
-      </c>
-      <c r="J14" s="3">
-        <v>8.6999999999999994E-2</v>
-      </c>
-      <c r="K14" s="4">
-        <v>7.4999999999999997E-2</v>
-      </c>
-      <c r="L14" s="9">
+        <v>9.2856999999999995E-2</v>
+      </c>
+      <c r="J14" s="1">
+        <v>8.7584800000000004E-2</v>
+      </c>
+      <c r="K14" s="1">
+        <v>5.9767679999999997E-2</v>
+      </c>
+      <c r="L14" s="5">
         <f t="shared" si="0"/>
-        <v>0.56730769230769229</v>
-      </c>
-      <c r="M14" s="14">
+        <v>0.66269663461538464</v>
+      </c>
+      <c r="M14" s="8">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="N14" s="14">
+        <v>0.89285576923076926</v>
+      </c>
+      <c r="N14" s="8">
         <f t="shared" si="2"/>
-        <v>0.83653846153846156</v>
-      </c>
-      <c r="O14" s="16">
+        <v>0.84216153846153852</v>
+      </c>
+      <c r="O14" s="10">
         <f t="shared" si="3"/>
-        <v>0.72115384615384615</v>
+        <v>0.57468923076923073</v>
       </c>
       <c r="P14" s="1">
         <f t="shared" si="4"/>
-        <v>-0.56730769230769229</v>
+        <v>0.23015913461538462</v>
       </c>
       <c r="Q14" s="1">
         <f t="shared" si="5"/>
-        <v>-0.11538461538461542</v>
-      </c>
-      <c r="R14" s="7" t="s">
-        <v>27</v>
+        <v>-0.26747230769230779</v>
+      </c>
+      <c r="R14" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15">
         <v>54.02</v>
       </c>
       <c r="C15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E15">
         <v>0.28599999999999998</v>
       </c>
-      <c r="F15">
+      <c r="F15" s="12">
         <v>0.44900000000000001</v>
       </c>
-      <c r="G15">
+      <c r="G15" s="12">
         <v>0.26400000000000001</v>
       </c>
-      <c r="H15" s="10">
-        <v>0.124</v>
+      <c r="H15" s="1">
+        <v>0.12371619</v>
       </c>
       <c r="I15" s="1">
-        <v>0.154</v>
-      </c>
-      <c r="J15" s="3">
-        <v>0.25700000000000001</v>
-      </c>
-      <c r="K15" s="4">
-        <v>0.16200000000000001</v>
-      </c>
-      <c r="L15" s="9">
+        <v>0.15419010999999999</v>
+      </c>
+      <c r="J15" s="1">
+        <v>0.2789855</v>
+      </c>
+      <c r="K15" s="1">
+        <v>0.16311523</v>
+      </c>
+      <c r="L15" s="5">
         <f t="shared" si="0"/>
-        <v>0.4335664335664336</v>
-      </c>
-      <c r="M15" s="14">
+        <v>0.43257409090909094</v>
+      </c>
+      <c r="M15" s="8">
         <f t="shared" si="1"/>
-        <v>0.53846153846153855</v>
-      </c>
-      <c r="N15" s="14">
+        <v>0.53912625874125875</v>
+      </c>
+      <c r="N15" s="8">
         <f t="shared" si="2"/>
-        <v>0.89860139860139865</v>
-      </c>
-      <c r="O15" s="16">
+        <v>0.97547377622377629</v>
+      </c>
+      <c r="O15" s="10">
         <f t="shared" si="3"/>
-        <v>0.56643356643356646</v>
+        <v>0.57033297202797206</v>
       </c>
       <c r="P15" s="1">
         <f t="shared" si="4"/>
-        <v>0.10489510489510495</v>
+        <v>0.10655216783216781</v>
       </c>
       <c r="Q15" s="3">
         <f t="shared" si="5"/>
-        <v>-0.33216783216783219</v>
-      </c>
-      <c r="R15" s="7" t="s">
-        <v>27</v>
+        <v>-0.40514080419580423</v>
+      </c>
+      <c r="R15" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16">
         <v>25.47</v>
       </c>
       <c r="C16" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D16" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E16">
         <v>0.19400000000000001</v>
       </c>
-      <c r="F16">
+      <c r="F16" s="12">
         <v>0.13600000000000001</v>
       </c>
-      <c r="G16">
+      <c r="G16" s="12">
         <v>0.11700000000000001</v>
       </c>
-      <c r="H16" s="10">
-        <v>0.161</v>
+      <c r="H16" s="1">
+        <v>0.16060537</v>
       </c>
       <c r="I16" s="1">
-        <v>0.17499999999999999</v>
-      </c>
-      <c r="J16" s="3">
-        <v>0.109</v>
-      </c>
-      <c r="K16" s="4">
-        <v>0.10199999999999999</v>
-      </c>
-      <c r="L16" s="9">
+        <v>0.17517506999999999</v>
+      </c>
+      <c r="J16" s="1">
+        <v>0.10861435999999999</v>
+      </c>
+      <c r="K16" s="1">
+        <v>0.10224854999999999</v>
+      </c>
+      <c r="L16" s="5">
         <f t="shared" si="0"/>
-        <v>0.82989690721649489</v>
-      </c>
-      <c r="M16" s="14">
+        <v>0.82786273195876281</v>
+      </c>
+      <c r="M16" s="8">
         <f t="shared" si="1"/>
-        <v>0.902061855670103</v>
-      </c>
-      <c r="N16" s="14">
+        <v>0.9029642783505154</v>
+      </c>
+      <c r="N16" s="8">
         <f t="shared" si="2"/>
-        <v>0.56185567010309279</v>
-      </c>
-      <c r="O16" s="16">
+        <v>0.55986783505154636</v>
+      </c>
+      <c r="O16" s="10">
         <f t="shared" si="3"/>
-        <v>0.52577319587628857</v>
+        <v>0.52705438144329897</v>
       </c>
       <c r="P16" s="1">
         <f t="shared" si="4"/>
-        <v>7.2164948453608102E-2</v>
+        <v>7.5101546391752594E-2</v>
       </c>
       <c r="Q16" s="1">
         <f t="shared" si="5"/>
-        <v>-3.6082474226804218E-2</v>
-      </c>
-      <c r="R16" s="7" t="s">
-        <v>27</v>
+        <v>-3.2813453608247389E-2</v>
+      </c>
+      <c r="R16" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B17">
         <v>26.14</v>
       </c>
       <c r="C17" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E17">
         <v>0.443</v>
       </c>
-      <c r="F17">
+      <c r="F17" s="12">
         <v>0.28299999999999997</v>
       </c>
-      <c r="G17">
+      <c r="G17" s="12">
         <v>0.249</v>
       </c>
-      <c r="H17" s="10">
-        <v>0.40699999999999997</v>
+      <c r="H17" s="1">
+        <v>0.40741717</v>
       </c>
       <c r="I17" s="1">
-        <v>0.378</v>
-      </c>
-      <c r="J17" s="3">
-        <v>0.26400000000000001</v>
-      </c>
-      <c r="K17" s="4">
-        <v>0.124</v>
-      </c>
-      <c r="L17" s="9">
+        <v>0.3780463</v>
+      </c>
+      <c r="J17" s="1">
+        <v>0.26349006000000003</v>
+      </c>
+      <c r="K17" s="1">
+        <v>0.12967835</v>
+      </c>
+      <c r="L17" s="5">
         <f t="shared" si="0"/>
-        <v>0.91873589164785541</v>
-      </c>
-      <c r="M17" s="14">
+        <v>0.91967758465011284</v>
+      </c>
+      <c r="M17" s="8">
         <f t="shared" si="1"/>
-        <v>0.85327313769751689</v>
-      </c>
-      <c r="N17" s="14">
+        <v>0.85337765237020313</v>
+      </c>
+      <c r="N17" s="8">
         <f t="shared" si="2"/>
-        <v>0.59593679458239279</v>
-      </c>
-      <c r="O17" s="16">
+        <v>0.59478568848758473</v>
+      </c>
+      <c r="O17" s="10">
         <f t="shared" si="3"/>
-        <v>0.27990970654627539</v>
+        <v>0.29272765237020315</v>
       </c>
       <c r="P17" s="1">
         <f t="shared" si="4"/>
-        <v>-6.5462753950338515E-2</v>
+        <v>-6.6299932279909712E-2</v>
       </c>
       <c r="Q17" s="1">
         <f t="shared" si="5"/>
-        <v>-0.3160270880361174</v>
-      </c>
-      <c r="R17" s="7" t="s">
-        <v>27</v>
+        <v>-0.30205803611738158</v>
+      </c>
+      <c r="R17" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B18">
         <v>26.14</v>
       </c>
       <c r="C18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D18" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E18">
         <v>0.30599999999999999</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="12">
         <v>0.24099999999999999</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="12">
         <v>0.217</v>
       </c>
-      <c r="H18" s="10">
-        <v>0.27</v>
+      <c r="H18" s="1">
+        <v>0.26986876999999998</v>
       </c>
       <c r="I18" s="1">
-        <v>0.27200000000000002</v>
-      </c>
-      <c r="J18" s="3">
-        <v>0.215</v>
-      </c>
-      <c r="K18" s="3">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="L18" s="9">
+        <v>0.27171289999999998</v>
+      </c>
+      <c r="J18" s="1">
+        <v>0.21478009000000001</v>
+      </c>
+      <c r="K18" s="1">
+        <v>0.19880328</v>
+      </c>
+      <c r="L18" s="5">
         <f t="shared" si="0"/>
-        <v>0.88235294117647067</v>
-      </c>
-      <c r="M18" s="14">
+        <v>0.88192408496732022</v>
+      </c>
+      <c r="M18" s="8">
         <f t="shared" si="1"/>
-        <v>0.88888888888888895</v>
-      </c>
-      <c r="N18" s="14">
+        <v>0.88795065359477121</v>
+      </c>
+      <c r="N18" s="8">
         <f t="shared" si="2"/>
-        <v>0.70261437908496738</v>
-      </c>
-      <c r="O18" s="16">
+        <v>0.7018957189542484</v>
+      </c>
+      <c r="O18" s="10">
         <f t="shared" si="3"/>
-        <v>0.65032679738562094</v>
+        <v>0.64968392156862742</v>
       </c>
       <c r="P18" s="1">
         <f t="shared" si="4"/>
-        <v>6.5359477124182774E-3</v>
+        <v>6.02656862745099E-3</v>
       </c>
       <c r="Q18" s="1">
         <f t="shared" si="5"/>
-        <v>-5.2287581699346442E-2</v>
-      </c>
-      <c r="R18" s="7" t="s">
-        <v>27</v>
+        <v>-5.2211797385620984E-2</v>
+      </c>
+      <c r="R18" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B19">
         <v>26.24</v>
       </c>
       <c r="C19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E19">
         <v>0.19900000000000001</v>
       </c>
-      <c r="F19">
+      <c r="F19" s="12">
         <v>0.188</v>
       </c>
-      <c r="G19">
+      <c r="G19" s="12">
         <v>0.158</v>
       </c>
-      <c r="H19" s="10">
-        <v>0.158</v>
+      <c r="H19" s="1">
+        <v>0.15799000999999999</v>
       </c>
       <c r="I19" s="1">
-        <v>0.123</v>
-      </c>
-      <c r="J19" s="3">
-        <v>0.13600000000000001</v>
-      </c>
-      <c r="K19" s="4">
-        <v>0.104</v>
-      </c>
-      <c r="L19" s="9">
+        <v>0.12305557</v>
+      </c>
+      <c r="J19" s="1">
+        <v>0.13571374999999999</v>
+      </c>
+      <c r="K19" s="1">
+        <v>0.10310506</v>
+      </c>
+      <c r="L19" s="5">
         <f t="shared" si="0"/>
-        <v>0.79396984924623115</v>
-      </c>
-      <c r="M19" s="14">
+        <v>0.79391964824120587</v>
+      </c>
+      <c r="M19" s="8">
         <f t="shared" si="1"/>
-        <v>0.61809045226130654</v>
-      </c>
-      <c r="N19" s="14">
+        <v>0.61836969849246226</v>
+      </c>
+      <c r="N19" s="8">
         <f t="shared" si="2"/>
-        <v>0.68341708542713564</v>
-      </c>
-      <c r="O19" s="16">
+        <v>0.68197864321608037</v>
+      </c>
+      <c r="O19" s="10">
         <f t="shared" si="3"/>
-        <v>0.5226130653266331</v>
+        <v>0.51811587939698489</v>
       </c>
       <c r="P19" s="1">
         <f t="shared" si="4"/>
-        <v>-0.17587939698492461</v>
+        <v>-0.17554994974874361</v>
       </c>
       <c r="Q19" s="1">
         <f t="shared" si="5"/>
-        <v>-0.16080402010050254</v>
-      </c>
-      <c r="R19" s="7" t="s">
-        <v>27</v>
+        <v>-0.16386276381909548</v>
+      </c>
+      <c r="R19" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20">
         <v>30.9</v>
       </c>
       <c r="C20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D20" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E20">
         <v>0.20399999999999999</v>
       </c>
-      <c r="F20">
+      <c r="F20" s="12">
         <v>0.183</v>
       </c>
-      <c r="G20">
+      <c r="G20" s="12">
         <v>0.17299999999999999</v>
       </c>
-      <c r="H20" s="10">
-        <v>0.14199999999999999</v>
+      <c r="H20" s="1">
+        <v>0.14162725000000001</v>
       </c>
       <c r="I20" s="1">
-        <v>0.107</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0.13700000000000001</v>
-      </c>
-      <c r="K20" s="4">
-        <v>9.1999999999999998E-2</v>
-      </c>
-      <c r="L20" s="9">
+        <v>0.10662772</v>
+      </c>
+      <c r="J20" s="1">
+        <v>0.13678246999999999</v>
+      </c>
+      <c r="K20" s="1">
+        <v>9.2511689999999994E-2</v>
+      </c>
+      <c r="L20" s="5">
         <f t="shared" si="0"/>
-        <v>0.69607843137254899</v>
-      </c>
-      <c r="M20" s="14">
+        <v>0.69425122549019613</v>
+      </c>
+      <c r="M20" s="8">
         <f t="shared" si="1"/>
-        <v>0.52450980392156865</v>
-      </c>
-      <c r="N20" s="14">
+        <v>0.52268490196078432</v>
+      </c>
+      <c r="N20" s="8">
         <f t="shared" si="2"/>
-        <v>0.67156862745098045</v>
-      </c>
-      <c r="O20" s="16">
+        <v>0.67050230392156862</v>
+      </c>
+      <c r="O20" s="10">
         <f t="shared" si="3"/>
-        <v>0.45098039215686275</v>
+        <v>0.45348867647058821</v>
       </c>
       <c r="P20" s="1">
         <f t="shared" si="4"/>
-        <v>-0.17156862745098034</v>
+        <v>-0.17156632352941181</v>
       </c>
       <c r="Q20" s="1">
         <f t="shared" si="5"/>
-        <v>-0.2205882352941177</v>
-      </c>
-      <c r="R20" s="7" t="s">
-        <v>27</v>
+        <v>-0.21701362745098041</v>
+      </c>
+      <c r="R20" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B21">
         <v>42.81</v>
       </c>
       <c r="C21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E21">
         <v>1.49</v>
       </c>
-      <c r="F21">
+      <c r="F21" s="12">
         <v>2.66</v>
       </c>
-      <c r="G21">
+      <c r="G21" s="12">
         <v>-2.1999999999999999E-2</v>
       </c>
-      <c r="H21" s="17">
-        <v>1.08</v>
-      </c>
-      <c r="I21" s="3">
-        <v>0.59199999999999997</v>
-      </c>
-      <c r="J21" s="19">
-        <v>1.69</v>
-      </c>
-      <c r="K21" s="4">
-        <v>-0.38400000000000001</v>
-      </c>
-      <c r="L21" s="9">
+      <c r="H21" s="1">
+        <v>1.07647648</v>
+      </c>
+      <c r="I21" s="1">
+        <v>0.59234383000000002</v>
+      </c>
+      <c r="J21" s="1">
+        <v>1.5348857899999999</v>
+      </c>
+      <c r="K21" s="1">
+        <v>-0.27529330000000002</v>
+      </c>
+      <c r="L21" s="5">
         <f t="shared" si="0"/>
-        <v>0.72483221476510074</v>
-      </c>
-      <c r="M21" s="14">
+        <v>0.72246743624161069</v>
+      </c>
+      <c r="M21" s="8">
         <f t="shared" si="1"/>
-        <v>0.3973154362416107</v>
-      </c>
-      <c r="N21" s="14">
+        <v>0.39754619463087248</v>
+      </c>
+      <c r="N21" s="8">
         <f t="shared" si="2"/>
-        <v>1.1342281879194631</v>
-      </c>
-      <c r="O21" s="16">
+        <v>1.0301246912751678</v>
+      </c>
+      <c r="O21" s="10">
         <f t="shared" si="3"/>
-        <v>-0.25771812080536916</v>
+        <v>-0.18476060402684566</v>
       </c>
       <c r="P21" s="1">
         <f>M21-L21</f>
-        <v>-0.32751677852349004</v>
+        <v>-0.32492124161073821</v>
       </c>
       <c r="Q21" s="3">
         <f t="shared" si="5"/>
-        <v>-1.3919463087248323</v>
-      </c>
-      <c r="R21" s="7" t="s">
-        <v>43</v>
+        <v>-1.2148852953020135</v>
+      </c>
+      <c r="R21" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B22">
         <v>42.81</v>
       </c>
       <c r="C22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E22">
         <v>3.42</v>
       </c>
-      <c r="F22" s="18">
+      <c r="F22" s="14">
         <v>1.4</v>
       </c>
-      <c r="G22">
+      <c r="G22" s="12">
         <v>1.19</v>
       </c>
-      <c r="H22" s="11">
-        <v>1.85</v>
+      <c r="H22" s="1">
+        <v>1.85236603</v>
       </c>
       <c r="I22" s="1">
-        <v>0.97799999999999998</v>
-      </c>
-      <c r="J22" s="3">
-        <v>0.80300000000000005</v>
-      </c>
-      <c r="K22" s="4">
-        <v>1.9E-2</v>
-      </c>
-      <c r="L22" s="9">
+        <v>0.97845227999999995</v>
+      </c>
+      <c r="J22" s="1">
+        <v>0.72324988999999995</v>
+      </c>
+      <c r="K22" s="1">
+        <v>0.12017439000000001</v>
+      </c>
+      <c r="L22" s="5">
         <f t="shared" si="0"/>
-        <v>0.54093567251461994</v>
-      </c>
-      <c r="M22" s="14">
+        <v>0.54162749415204681</v>
+      </c>
+      <c r="M22" s="8">
         <f t="shared" si="1"/>
-        <v>0.28596491228070176</v>
-      </c>
-      <c r="N22" s="14">
+        <v>0.28609715789473683</v>
+      </c>
+      <c r="N22" s="8">
         <f t="shared" si="2"/>
-        <v>0.23479532163742692</v>
-      </c>
-      <c r="O22" s="16">
+        <v>0.21147657602339182</v>
+      </c>
+      <c r="O22" s="10">
         <f t="shared" si="3"/>
-        <v>5.5555555555555558E-3</v>
+        <v>3.5138710526315793E-2</v>
       </c>
       <c r="P22" s="1">
         <f t="shared" si="4"/>
-        <v>-0.25497076023391818</v>
+        <v>-0.25553033625730998</v>
       </c>
       <c r="Q22" s="1">
         <f t="shared" si="5"/>
-        <v>-0.22923976608187135</v>
-      </c>
-      <c r="R22" s="7" t="s">
-        <v>27</v>
+        <v>-0.17633786549707603</v>
+      </c>
+      <c r="R22" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B23">
         <v>35.270000000000003</v>
       </c>
       <c r="C23" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E23">
         <v>0.33200000000000002</v>
       </c>
-      <c r="F23">
+      <c r="F23" s="12">
         <v>0.38400000000000001</v>
       </c>
-      <c r="G23">
+      <c r="G23" s="12">
         <v>0.39300000000000002</v>
       </c>
-      <c r="H23" s="10">
-        <v>0.188</v>
+      <c r="H23" s="1">
+        <v>0.18836463000000001</v>
       </c>
       <c r="I23" s="1">
-        <v>0.252</v>
+        <v>0.25241818999999999</v>
       </c>
       <c r="J23" s="1">
-        <v>0.16600000000000001</v>
-      </c>
-      <c r="K23">
-        <v>0.248</v>
-      </c>
-      <c r="L23" s="9">
+        <v>0.16610628999999999</v>
+      </c>
+      <c r="K23" s="1">
+        <v>0.24560271</v>
+      </c>
+      <c r="L23" s="5">
         <f t="shared" si="0"/>
-        <v>0.56626506024096379</v>
-      </c>
-      <c r="M23" s="14">
+        <v>0.56736334337349392</v>
+      </c>
+      <c r="M23" s="8">
         <f t="shared" si="1"/>
-        <v>0.75903614457831325</v>
-      </c>
-      <c r="N23" s="14">
+        <v>0.7602957530120481</v>
+      </c>
+      <c r="N23" s="8">
         <f t="shared" si="2"/>
-        <v>0.5</v>
-      </c>
-      <c r="O23" s="16">
+        <v>0.50032015060240953</v>
+      </c>
+      <c r="O23" s="10">
         <f t="shared" si="3"/>
-        <v>0.74698795180722888</v>
+        <v>0.73976719879518071</v>
       </c>
       <c r="P23" s="1">
         <f t="shared" si="4"/>
-        <v>0.19277108433734946</v>
+        <v>0.19293240963855418</v>
       </c>
       <c r="Q23" s="1">
         <f t="shared" si="5"/>
-        <v>0.24698795180722888</v>
-      </c>
-      <c r="R23" s="7" t="s">
-        <v>27</v>
+        <v>0.23944704819277118</v>
+      </c>
+      <c r="R23" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B24">
         <v>36.07</v>
       </c>
       <c r="C24" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E24">
         <v>0.39700000000000002</v>
       </c>
-      <c r="F24">
+      <c r="F24" s="12">
         <v>0.34399999999999997</v>
       </c>
-      <c r="G24">
+      <c r="G24" s="12">
         <v>0.376</v>
       </c>
-      <c r="H24" s="10">
-        <v>0.249</v>
+      <c r="H24" s="1">
+        <v>0.24932330999999999</v>
       </c>
       <c r="I24" s="1">
-        <v>0.24</v>
+        <v>0.23971513</v>
       </c>
       <c r="J24" s="1">
-        <v>0.215</v>
-      </c>
-      <c r="K24">
-        <v>0.224</v>
-      </c>
-      <c r="L24" s="9">
+        <v>0.22804624000000001</v>
+      </c>
+      <c r="K24" s="1">
+        <v>0.23414782000000001</v>
+      </c>
+      <c r="L24" s="5">
         <f t="shared" si="0"/>
-        <v>0.62720403022670024</v>
-      </c>
-      <c r="M24" s="14">
+        <v>0.62801841309823669</v>
+      </c>
+      <c r="M24" s="8">
         <f t="shared" si="1"/>
-        <v>0.60453400503778332</v>
-      </c>
-      <c r="N24" s="14">
+        <v>0.60381644836272041</v>
+      </c>
+      <c r="N24" s="8">
         <f t="shared" si="2"/>
-        <v>0.54156171284634758</v>
-      </c>
-      <c r="O24" s="16">
+        <v>0.57442377833753144</v>
+      </c>
+      <c r="O24" s="10">
         <f t="shared" si="3"/>
-        <v>0.5642317380352645</v>
+        <v>0.58979299748110825</v>
       </c>
       <c r="P24" s="1">
         <f t="shared" si="4"/>
-        <v>-2.267002518891692E-2</v>
+        <v>-2.4201964735516279E-2</v>
       </c>
       <c r="Q24" s="1">
         <f t="shared" si="5"/>
-        <v>2.267002518891692E-2</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>27</v>
+        <v>1.5369219143576807E-2</v>
+      </c>
+      <c r="R24" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B25">
         <v>42.42</v>
       </c>
       <c r="C25" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D25" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E25">
         <v>0.46400000000000002</v>
       </c>
-      <c r="F25">
+      <c r="F25" s="12">
         <v>0.45400000000000001</v>
       </c>
-      <c r="G25">
+      <c r="G25" s="12">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="H25" s="10">
-        <v>0.25800000000000001</v>
+      <c r="H25" s="1">
+        <v>0.25770731000000002</v>
       </c>
       <c r="I25" s="1">
-        <v>4.4999999999999998E-2</v>
+        <v>4.5339400000000002E-2</v>
       </c>
       <c r="J25" s="1">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="K25">
-        <v>-4.9000000000000002E-2</v>
-      </c>
-      <c r="L25" s="9">
+        <v>0.31192150000000002</v>
+      </c>
+      <c r="K25" s="1">
+        <v>-1.41656E-2</v>
+      </c>
+      <c r="L25" s="5">
         <f t="shared" si="0"/>
-        <v>0.55603448275862066</v>
-      </c>
-      <c r="M25" s="14">
+        <v>0.55540368534482765</v>
+      </c>
+      <c r="M25" s="8">
         <f t="shared" si="1"/>
-        <v>9.6982758620689641E-2</v>
-      </c>
-      <c r="N25" s="14">
+        <v>9.771422413793103E-2</v>
+      </c>
+      <c r="N25" s="8">
         <f t="shared" si="2"/>
-        <v>0.62284482758620685</v>
-      </c>
-      <c r="O25" s="16">
+        <v>0.67224461206896557</v>
+      </c>
+      <c r="O25" s="10">
         <f t="shared" si="3"/>
-        <v>-0.10560344827586207</v>
+        <v>-3.0529310344827587E-2</v>
       </c>
       <c r="P25" s="1">
         <f t="shared" si="4"/>
-        <v>-0.45905172413793105</v>
+        <v>-0.45768946120689663</v>
       </c>
       <c r="Q25" s="1">
         <f t="shared" si="5"/>
-        <v>-0.72844827586206895</v>
-      </c>
-      <c r="R25" s="7" t="s">
-        <v>43</v>
+        <v>-0.70277392241379322</v>
+      </c>
+      <c r="R25" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B26">
         <v>38.93</v>
       </c>
       <c r="C26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D26" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E26">
         <v>0.13900000000000001</v>
       </c>
-      <c r="F26">
+      <c r="F26" s="12">
         <v>0.14399999999999999</v>
       </c>
-      <c r="G26">
+      <c r="G26" s="12">
         <v>-2.9000000000000001E-2</v>
       </c>
-      <c r="H26" s="10">
-        <v>7.3999999999999996E-2</v>
+      <c r="H26" s="1">
+        <v>7.3876769999999994E-2</v>
       </c>
       <c r="I26" s="1">
-        <v>-0.192</v>
+        <v>-0.19248870000000001</v>
       </c>
       <c r="J26" s="1">
-        <v>5.7000000000000002E-2</v>
-      </c>
-      <c r="K26">
-        <v>-5.8999999999999997E-2</v>
-      </c>
-      <c r="L26" s="9">
+        <v>8.6571110000000007E-2</v>
+      </c>
+      <c r="K26" s="1">
+        <v>-8.3204999999999998E-3</v>
+      </c>
+      <c r="L26" s="5">
         <f t="shared" si="0"/>
-        <v>0.53237410071942437</v>
-      </c>
-      <c r="M26" s="14">
+        <v>0.53148755395683445</v>
+      </c>
+      <c r="M26" s="8">
         <f t="shared" si="1"/>
-        <v>-1.3812949640287768</v>
-      </c>
-      <c r="N26" s="14">
+        <v>-1.3848107913669065</v>
+      </c>
+      <c r="N26" s="8">
         <f t="shared" si="2"/>
-        <v>0.41007194244604317</v>
-      </c>
-      <c r="O26" s="16">
+        <v>0.62281374100719422</v>
+      </c>
+      <c r="O26" s="10">
         <f t="shared" si="3"/>
-        <v>-0.42446043165467617</v>
+        <v>-5.9859712230215821E-2</v>
       </c>
       <c r="P26" s="3">
         <f>M26-L26</f>
-        <v>-1.9136690647482011</v>
+        <v>-1.916298345323741</v>
       </c>
       <c r="Q26" s="1">
         <f>O26-N26</f>
-        <v>-0.83453237410071934</v>
-      </c>
-      <c r="R26" s="7" t="s">
-        <v>43</v>
+        <v>-0.68267345323741002</v>
+      </c>
+      <c r="R26" s="4" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B27">
         <v>38.93</v>
       </c>
       <c r="C27" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D27" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E27">
         <v>0.29899999999999999</v>
       </c>
-      <c r="F27" s="1">
+      <c r="F27" s="13">
         <v>0.34</v>
       </c>
-      <c r="G27">
+      <c r="G27" s="12">
         <v>-2.9000000000000001E-2</v>
       </c>
-      <c r="H27" s="10">
-        <v>0.16700000000000001</v>
+      <c r="H27" s="1">
+        <v>0.1673993</v>
       </c>
       <c r="I27" s="1">
-        <v>-0.186</v>
+        <v>-0.1863119</v>
       </c>
       <c r="J27" s="1">
-        <v>0.19900000000000001</v>
-      </c>
-      <c r="K27">
-        <v>-7.9000000000000001E-2</v>
-      </c>
-      <c r="L27" s="9">
+        <v>0.20265747000000001</v>
+      </c>
+      <c r="K27" s="1">
+        <v>7.2774749999999999E-2</v>
+      </c>
+      <c r="L27" s="5">
         <f t="shared" si="0"/>
-        <v>0.55852842809364556</v>
-      </c>
-      <c r="M27" s="14">
+        <v>0.55986387959866224</v>
+      </c>
+      <c r="M27" s="8">
         <f t="shared" si="1"/>
-        <v>-0.62207357859531776</v>
-      </c>
-      <c r="N27" s="14">
+        <v>-0.62311672240802674</v>
+      </c>
+      <c r="N27" s="8">
         <f t="shared" si="2"/>
-        <v>0.66555183946488305</v>
-      </c>
-      <c r="O27" s="16">
+        <v>0.67778418060200674</v>
+      </c>
+      <c r="O27" s="10">
         <f t="shared" si="3"/>
-        <v>-0.26421404682274247</v>
+        <v>0.2433938127090301</v>
       </c>
       <c r="P27" s="1">
         <f t="shared" si="4"/>
-        <v>-1.1806020066889633</v>
+        <v>-1.1829806020066891</v>
       </c>
       <c r="Q27" s="1">
         <f t="shared" si="5"/>
-        <v>-0.92976588628762546</v>
-      </c>
-      <c r="R27" s="7" t="s">
-        <v>43</v>
+        <v>-0.43439036789297664</v>
+      </c>
+      <c r="R27" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28">
         <v>38.93</v>
       </c>
       <c r="C28" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D28" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="E28">
         <v>0.35699999999999998</v>
       </c>
-      <c r="F28" s="1">
+      <c r="F28" s="13">
         <v>0.48</v>
       </c>
-      <c r="G28">
+      <c r="G28" s="12">
         <v>0.38800000000000001</v>
       </c>
-      <c r="H28" s="10">
-        <v>0.21199999999999999</v>
+      <c r="H28" s="1">
+        <v>0.21176983999999999</v>
       </c>
       <c r="I28" s="1">
-        <v>0.11799999999999999</v>
+        <v>0.11763234</v>
       </c>
       <c r="J28" s="1">
-        <v>0.27200000000000002</v>
+        <v>0.28759375999999998</v>
       </c>
       <c r="K28" s="1">
-        <v>9.2999999999999999E-2</v>
-      </c>
-      <c r="L28" s="9">
+        <v>8.8655319999999996E-2</v>
+      </c>
+      <c r="L28" s="5">
         <f t="shared" si="0"/>
-        <v>0.5938375350140056</v>
-      </c>
-      <c r="M28" s="14">
+        <v>0.59319282913165261</v>
+      </c>
+      <c r="M28" s="8">
         <f t="shared" si="1"/>
-        <v>0.33053221288515405</v>
-      </c>
-      <c r="N28" s="14">
+        <v>0.32950235294117647</v>
+      </c>
+      <c r="N28" s="8">
         <f t="shared" si="2"/>
-        <v>0.76190476190476197</v>
-      </c>
-      <c r="O28" s="16">
+        <v>0.80558476190476191</v>
+      </c>
+      <c r="O28" s="10">
         <f t="shared" si="3"/>
-        <v>0.26050420168067229</v>
+        <v>0.24833422969187674</v>
       </c>
       <c r="P28" s="1">
         <f t="shared" si="4"/>
-        <v>-0.26330532212885155</v>
+        <v>-0.26369047619047614</v>
       </c>
       <c r="Q28" s="1">
         <f t="shared" si="5"/>
-        <v>-0.50140056022408963</v>
-      </c>
-      <c r="R28" s="7" t="s">
-        <v>27</v>
+        <v>-0.55725053221288512</v>
+      </c>
+      <c r="R28" s="4" t="s">
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Produced figures for TPC vs DDE model comparison
</commit_message>
<xml_diff>
--- a/Model results Tave.xlsx
+++ b/Model results Tave.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnson/Documents/Christopher/GitHub/Johnson_Insect_Responses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81323491-6865-3041-9322-6A7D6F10FC55}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CF05DB8-9ECE-7748-AF6A-E842FCF61E8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1880" yWindow="500" windowWidth="26880" windowHeight="13100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1115,9 +1115,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2474,7 +2474,7 @@
         <v>-0.17633786549707603</v>
       </c>
       <c r="R22" s="4" t="s">
-        <v>26</v>
+        <v>42</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.2">

</xml_diff>